<commit_message>
Fix a person's caption in multi feature
</commit_message>
<xml_diff>
--- a/loadDatabase/religion/святые.xlsx
+++ b/loadDatabase/religion/святые.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$V$135</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2003" uniqueCount="1361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2004" uniqueCount="1362">
   <si>
     <t>Фамилия</t>
   </si>
@@ -5194,6 +5194,9 @@
 Очевидцами мученической смерти святителя были 20 французских моряков, реакцию которых описал французский писатель Рене Пуо. Французский патруль наблюдал… Французские моряки «были вне себя». Без всякого преувеличения, они дрожали от гнева и решили вмешаться. Однако начальствовавший над ними офицер, следуя данному ему приказу, с пистолетом в руке помешал им что-либо предпринять…
 Трагическая смерть настигла большое число выдающихся греков Смирны, представителей греческой общины, священников, учителей и старейшин, которые отказались бежать и пали вместе с беззащитным безоружным населением. Вместе с Хризостомом турки уничтожили 347 священников Смирнской епархии из общего числа 459, а также митрополитов Мосхонисийского Амвросия, Кидонийского Григория – погребенного заживо, Иконийского Зилона – зарезанного. Из 46 церквей Смирны сохранилось только три. Никому не удалось узнать, что осталось от растерзанного тела святителя Хризостома. По слухам, тем не менее, тело было похоронено на участке земли, принадлежавшем спортивному обществу Аполлона, а по другой версии – близ одной реки…
 В 1992 году по инициативе афинского Союза смирнийцев Священный Синод Элладской Церкви причислил митрополита Хризостома к лику святых. Указом 2556/5-7 от 1993 года Священный Синод Константинопольской Православной Церкви установил празднование Новомучеников Малоазийской катастрофы в воскресенье предшествующее Крестовоздвижению и поставил имя священномученика Хризостома во главе этого сонма святых.</t>
+  </si>
+  <si>
+    <t>14.07.1901</t>
   </si>
 </sst>
 </file>
@@ -5739,9 +5742,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V137"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R31" sqref="R31"/>
+    <sheetView showFormulas="1" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12244,8 +12247,8 @@
       <c r="C120" s="22" t="s">
         <v>889</v>
       </c>
-      <c r="D120" s="24">
-        <v>561</v>
+      <c r="D120" s="24" t="s">
+        <v>1361</v>
       </c>
       <c r="E120" s="22" t="s">
         <v>887</v>

</xml_diff>

<commit_message>
Fix temples error Reload all images for temples and persons
</commit_message>
<xml_diff>
--- a/loadDatabase/religion/святые.xlsx
+++ b/loadDatabase/religion/святые.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="587"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" tabRatio="587"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -13,8 +13,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$V$141</definedName>
   </definedNames>
   <calcPr calcId="124519" refMode="R1C1"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -4596,27 +4596,9 @@
     <t>https://drevo-info.ru/images/003/010164.jpg</t>
   </si>
   <si>
-    <t>http://www.eparhia-ufa.ru/sites/default/files/5082_averkiy_severovostokov.jpg</t>
-  </si>
-  <si>
-    <t>http://www.eparhia-ufa.ru/sites/default/files/_1_1_0.jpg</t>
-  </si>
-  <si>
     <t>https://upload.wikimedia.org/wikipedia/ru/6/63/StVarvara.jpg</t>
   </si>
   <si>
-    <t>http://www.eparhia-ufa.ru/sites/default/files/18_evgraf-evarestov_0.jpg</t>
-  </si>
-  <si>
-    <t>http://www.eparhia-ufa.ru/sites/default/files/full_1224529327.jpg</t>
-  </si>
-  <si>
-    <t>http://www.eparhia-ufa.ru/sites/default/files/bkeoacwr6gi.jpg</t>
-  </si>
-  <si>
-    <t>http://www.eparhia-ufa.ru/sites/default/files/_20120206_2003763905.jpg</t>
-  </si>
-  <si>
     <t>https://upload.wikimedia.org/wikipedia/ru/1/1d/O_moiseychigvintsev.jpg</t>
   </si>
   <si>
@@ -4626,9 +4608,6 @@
     <t>https://upload.wikimedia.org/wikipedia/commons/2/2c/Bishop_Simeon_Shleev.jpg</t>
   </si>
   <si>
-    <t>http://www.eparhia-ufa.ru/sites/default/files/timofey_petropavlovskiy_sshchmch_0.jpg</t>
-  </si>
-  <si>
     <t>https://upload.wikimedia.org/wikipedia/commons/8/80/Mitropolitan_Alexis_by_G.Zinovyev_%281690s%2C_GTG%29.jpg</t>
   </si>
   <si>
@@ -4713,9 +4692,6 @@
     <t>https://azbyka.ru/days/assets/img/saints/4646/p1ac4r7o9o181e1sd2sgrujo16no3.png</t>
   </si>
   <si>
-    <t>https://lh3.googleusercontent.com/xUvgoz7UsOK7WoBwvwt-aSrT07_BR3nBROqC1OhfqUCGrC-Wz7m4jCfppLXPty_SzOLy94Y9LA0fP3AqTnJwOPp6tdznHOgux7BjABqgyi4CX0ZLIA3pjiS5b95F9LEmkDH18oAd-DoA_g-twZJRWeh9RAmkyty9n_NGIzpjJ22XETLkHf6PW0i3cA4Z-fLa1Q1P2XMdAM2XmfwBGPo6WYxLaTE9fUmXRJzqKhheDzLL1gvvO-ZCk6h5MOeik_5RW3ys253b6VNgzYs1VhL1B8pBFknsW_LO5GVj_e305Be0hAKJC318-unt4kb2WZ9gs4di9gv5Zn5UWd3QzQ9Tl4zJ6AQTnKypydhRi1zaRzWmxwR_ew9jJVDsZrbHdLbdZPI75qF81-cHhh9fS2qTZd-UV1pCJpnyXZoIMyjxHig9_P87xnsxFiD27PHDXgd8RxlzZQPFp_KMgX5Oj0p9khKBXVOSFyPgH7s9HHcfQWt-tjc3nZON5L_34X8CRA01d4YVXoIknouXuiH_g14Fnh0WKDxHuYI3NyMbuabJdCoZx37WzX9guqbwXNo0ljc5C6byr7-pfWqBwQ_7MS5V9ipXIUdN239LTwjX1fs5G6rKGtvN4nNRThud737niJZ1IdBCXcmkiWlX11g02rTsGRwbT2NLujQO=w520-h150-no</t>
-  </si>
-  <si>
     <t>https://upload.wikimedia.org/wikipedia/commons/1/14/%D0%9F%D1%80%D0%BF._%D0%90%D0%BD%D1%82%D0%BE%D0%BD%D0%B8%D0%B9_%D0%9A%D1%80%D0%B0%D1%81%D0%BD%D0%BE%D1%85%D0%BE%D0%BB%D0%BC%D1%81%D0%BA%D0%B8%D0%B9.jpg</t>
   </si>
   <si>
@@ -5073,9 +5049,6 @@
     <t>Архиепископство, мученичество</t>
   </si>
   <si>
-    <t>https://www.google.com/search?q=%D0%B0%D0%BB%D0%B5%D0%BA%D1%81%D0%B0%D0%BD%D0%B4%D1%80+%D1%84%D0%B5%D0%BE%D1%84%D0%B0%D0%BD%D0%BE%D0%B2%D0%B8%D1%87+%D0%BF%D0%B5%D1%82%D1%80%D0%BE%D0%B2%D1%81%D0%BA%D0%B8%D0%B9&amp;sxsrf=ALeKk035AKkHbB-5Ge59CsuLdtVHUQrOIQ:1612688437485&amp;tbm=isch&amp;source=iu&amp;ictx=1&amp;fir=xVDKnUMpF29aiM%252CxpwqsKPZlXDbhM%252C_&amp;vet=1&amp;usg=AI4_-kQ7s-J3YygphSvOGvJ1dO_To65yzg&amp;sa=X&amp;ved=2ahUKEwi9_8vLtNfuAhXrmIsKHVtfD7UQ9QF6BAgJEAE#imgrc=xVDKnUMpF29aiM</t>
-  </si>
-  <si>
     <t>Ястребов</t>
   </si>
   <si>
@@ -5103,9 +5076,6 @@
     <t>https://ru.wikipedia.org/wiki/%D0%98%D0%BD%D0%BD%D0%BE%D0%BA%D0%B5%D0%BD%D1%82%D0%B8%D0%B9_(%D0%AF%D1%81%D1%82%D1%80%D0%B5%D0%B1%D0%BE%D0%B2)</t>
   </si>
   <si>
-    <t>https://commons.wikimedia.org/wiki/File:%D0%95%D0%BF%D0%B8%D1%81%D0%BA%D0%BE%D0%BF_%D0%9A%D0%B0%D0%BD%D0%B5%D0%B2%D1%81%D0%BA%D0%B8%D0%B9_%D0%98%D0%BD%D0%BD%D0%BE%D0%BA%D0%B5%D0%BD%D1%82%D0%B8%D0%B9.jpg?uselang=ru</t>
-  </si>
-  <si>
     <t>г. Москва</t>
   </si>
   <si>
@@ -5136,9 +5106,6 @@
     <t>https://bessmertnybarak.ru/Buzov_Iosif_Petrovich/</t>
   </si>
   <si>
-    <t>https://lh3.googleusercontent.com/MN7VbtAMfrEDV-RZR0l234bPbEGoK3tsFwG1Kl_SlxYlFapV78pRk5Jgkt0nAgiqvx-jtR4=s85</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ермаков </t>
   </si>
   <si>
@@ -5158,9 +5125,6 @@
   </si>
   <si>
     <t>Родился 31/07/1862 в Санкт-Петербурге. Окончил Киевскую духовную академию. В 1887 г пострижен в моншество и посвящен в сан иеромонаха. На протяжении 11 лет преподавал в духовных учебных заведениях.</t>
-  </si>
-  <si>
-    <t>https://commons.wikimedia.org/wiki/File:%D0%9C%D0%B8%D1%85%D0%B0%D0%B8%D0%BB_(%D0%95%D1%80%D0%BC%D0%B0%D0%BA%D0%BE%D0%B2).jpg?uselang=ru</t>
   </si>
   <si>
     <t>06.10</t>
@@ -5508,20 +5472,56 @@
     <t>Ярославль</t>
   </si>
   <si>
-    <t xml:space="preserve">https://yargid.ru/uploads/images/00/00/01/2014/11/10/eaa208.jpg </t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ru.wikipedia.org/wiki/Фёдор_Ростиславич_Чёрный </t>
   </si>
   <si>
     <t>Фёдор Ростисла́вич Чёрный (Чермный) (около 1240 или 1 сентября 1233 — 1299) — князь ярославский, можайский и великий князь смоленский. Прозвище Чермный означает как рыжий, так и красивый. В период с не ранее 1266 по 1276 год, возможно, пребывал в Золотой Орде, где, по легенде, по мнению Евгения Ермолина, его полюбила ханша Джиджекхатунь и благоволил хан Менгу-Тимур, они сватали свою дочь за него, несмотря на живую жену. Анастасия вскоре умерла, Фёдор пытался вернуться в Ярославль, но этому воспротивилась княгиня Ксения с боярами, объявившие князем малолетнего Михаила. Фёдор, оставшись в Орде, женился второй раз, на дочери хана, в православии Анне, получив за неё большое приданое (36 городов) и большой почёт у монголов. Родились сыновья Давид и Константин, в то время как старший сын Михаил умер в Ярославле. После этого Фёдор с семьёй отъехал в Ярославль с ханским ярлыком на княжение.</t>
+  </si>
+  <si>
+    <t>http://www.rlib.yar.ru/_yar_bibliography/photo/04/02_02.jpg</t>
+  </si>
+  <si>
+    <t>http://www.logoslovo.ru/media/pic_middle/21/64633.jpg</t>
+  </si>
+  <si>
+    <t>http://xram-kusa.cerkov.ru/files/2018/02/%D1%81%D0%B2%D1%89.%D0%BC%D1%87.%D0%90%D0%BB%D0%B5%D0%BA%D1%81%D0%B8%D0%B9-%D0%9A%D0%B0%D0%BD%D1%86%D0%B5%D1%80%D0%BE%D0%B2-2.jpg</t>
+  </si>
+  <si>
+    <t>https://drevo-info.ru/images/002/007795.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/ru/7/78/JatsenkoK.jpg</t>
+  </si>
+  <si>
+    <t>https://ic.pics.livejournal.com/kostryukov/41217450/122066/122066_original.jpg</t>
+  </si>
+  <si>
+    <t>https://www.pravchelny.ru/www/images/2013/8/margarita_431.jpg</t>
+  </si>
+  <si>
+    <t>https://azbyka.ru/days/assets/img/saints/201/p1e05mhrq4195kr03nvm183eigv5.jpg</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/xUvgoz7UsOK7WoBwvwt-aSrT07_BR3nBROqC1OhfqUCGrC-Wz7m4jCfppLXPty_SzOLy94Y9LA0fP3AqTnJwOPp6tdznHOgux7BjABqgyi4CX0ZLIA3pjiS5b95F9LEmkDH18oAd-DoA_g-twZJRWeh9RAmkyty9n_NGIzpjJ22XETLkHf6PW0i3cA4Z-fLa1Q1P2XMdAM2XmfwBGPo6WYxLaTE9fUmXRJzqKhheDzLL1gvvO-ZCk6h5MOeik_5RW3ys253b6VNgzYs1VhL1B8pBFknsW_LO5GVj_e305Be0hAKJC318-unt4kb2WZ9gs4di9gv5Zn5UWd3QzQ9Tl4zJ6AQTnKypydhRi1zaRzWmxwR_ew9jJVDsZrbHdLbdZPI75qF81-cHhh9fS2qTZd-UV1pCJpnyXZoIMyjxHig9_P87xnsxFiD27PHDXgd8RxlzZQPFp_KMgX5Oj0p9khKBXVOSFyPgH7s9HHcfQWt-tjc3nZON5L_34X8CRA01d4YVXoIknouXuiH_g14Fnh0WKDxHuYI3NyMbuabJdCoZx37WzX9guqbwXNo0ljc5C6byr7-pfWqBwQ_7MS5V9ipXIUdN239LTwjX1fs5G6rKGtvN4nNRThud737niJZ1IdBCXcmkiWlX11g02rTsGRwbT2NLujQO=w520-h739-no</t>
+  </si>
+  <si>
+    <t>https://bessmertnybarak.ru/filesSt/2294_Buzov_Iosif_Petrovich/foto_1445330877.jpg</t>
+  </si>
+  <si>
+    <t>http://213.171.53.29/foto_1/ob7-21a.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/4/49/%D0%95%D0%BF%D0%B8%D1%81%D0%BA%D0%BE%D0%BF_%D0%9A%D0%B0%D0%BD%D0%B5%D0%B2%D1%81%D0%BA%D0%B8%D0%B9_%D0%98%D0%BD%D0%BD%D0%BE%D0%BA%D0%B5%D0%BD%D1%82%D0%B8%D0%B9.jpg?uselang=ru</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/8/8e/%D0%9C%D0%B8%D1%85%D0%B0%D0%B8%D0%BB_%28%D0%95%D1%80%D0%BC%D0%B0%D0%BA%D0%BE%D0%B2%29.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5707,7 +5707,7 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5810,6 +5810,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -5873,7 +5874,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -5908,7 +5909,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -6085,22 +6086,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V141"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H138" sqref="H138"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T146" sqref="T146"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="24.95" customHeight="1"/>
   <cols>
     <col min="1" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" style="3" customWidth="1"/>
@@ -6119,7 +6120,7 @@
     <col min="22" max="22" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="24.95" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6163,7 +6164,7 @@
         <v>9</v>
       </c>
       <c r="O1" t="s">
-        <v>1231</v>
+        <v>1223</v>
       </c>
       <c r="P1" s="40" t="s">
         <v>10</v>
@@ -6187,7 +6188,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="24.95" customHeight="1">
       <c r="B2" t="s">
         <v>17</v>
       </c>
@@ -6216,7 +6217,7 @@
         <v>33</v>
       </c>
       <c r="P2" s="40" t="s">
-        <v>1234</v>
+        <v>1226</v>
       </c>
       <c r="Q2" t="s">
         <v>23</v>
@@ -6234,7 +6235,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="24.95" customHeight="1">
       <c r="B3" t="s">
         <v>25</v>
       </c>
@@ -6266,10 +6267,10 @@
         <v>26</v>
       </c>
       <c r="O3" s="38" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P3" s="40" t="s">
-        <v>1235</v>
+        <v>1227</v>
       </c>
       <c r="Q3" t="s">
         <v>27</v>
@@ -6287,7 +6288,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="24.95" customHeight="1">
       <c r="B4" t="s">
         <v>31</v>
       </c>
@@ -6310,7 +6311,7 @@
         <v>33</v>
       </c>
       <c r="P4" s="40" t="s">
-        <v>1236</v>
+        <v>1228</v>
       </c>
       <c r="Q4" t="s">
         <v>23</v>
@@ -6328,7 +6329,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="24.95" customHeight="1">
       <c r="B5" t="s">
         <v>37</v>
       </c>
@@ -6375,7 +6376,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="24.95" customHeight="1">
       <c r="B6" t="s">
         <v>45</v>
       </c>
@@ -6419,7 +6420,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="24.95" customHeight="1">
       <c r="B7" t="s">
         <v>51</v>
       </c>
@@ -6448,7 +6449,7 @@
         <v>53</v>
       </c>
       <c r="P7" s="40" t="s">
-        <v>1237</v>
+        <v>1229</v>
       </c>
       <c r="Q7" t="s">
         <v>56</v>
@@ -6466,7 +6467,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="24.95" customHeight="1">
       <c r="B8" t="s">
         <v>58</v>
       </c>
@@ -6507,7 +6508,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="24.95" customHeight="1">
       <c r="B9" t="s">
         <v>62</v>
       </c>
@@ -6530,7 +6531,7 @@
         <v>53</v>
       </c>
       <c r="P9" s="40" t="s">
-        <v>1238</v>
+        <v>1230</v>
       </c>
       <c r="Q9" t="s">
         <v>56</v>
@@ -6548,7 +6549,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="24.95" customHeight="1">
       <c r="B10" t="s">
         <v>67</v>
       </c>
@@ -6598,7 +6599,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="24.95" customHeight="1">
       <c r="B11" t="s">
         <v>72</v>
       </c>
@@ -6621,10 +6622,10 @@
         <v>73</v>
       </c>
       <c r="O11" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P11" s="40" t="s">
-        <v>1239</v>
+        <v>1231</v>
       </c>
       <c r="Q11" t="s">
         <v>74</v>
@@ -6645,7 +6646,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="24.95" customHeight="1">
       <c r="B12" t="s">
         <v>78</v>
       </c>
@@ -6668,7 +6669,7 @@
         <v>53</v>
       </c>
       <c r="P12" s="40" t="s">
-        <v>1240</v>
+        <v>1232</v>
       </c>
       <c r="Q12" t="s">
         <v>56</v>
@@ -6686,7 +6687,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="24.95" customHeight="1">
       <c r="B13" t="s">
         <v>82</v>
       </c>
@@ -6706,7 +6707,7 @@
         <v>84</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>1233</v>
+        <v>1225</v>
       </c>
       <c r="M13" s="3" t="s">
         <v>1080</v>
@@ -6718,7 +6719,7 @@
         <v>26</v>
       </c>
       <c r="P13" s="40" t="s">
-        <v>1241</v>
+        <v>1233</v>
       </c>
       <c r="Q13" t="s">
         <v>85</v>
@@ -6730,16 +6731,16 @@
         <v>87</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>1317</v>
+        <v>1309</v>
       </c>
       <c r="U13" s="3" t="s">
-        <v>1304</v>
+        <v>1296</v>
       </c>
       <c r="V13" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="24.95" customHeight="1">
       <c r="B14" t="s">
         <v>88</v>
       </c>
@@ -6765,7 +6766,7 @@
         <v>33</v>
       </c>
       <c r="P14" s="40" t="s">
-        <v>1243</v>
+        <v>1235</v>
       </c>
       <c r="Q14" t="s">
         <v>91</v>
@@ -6777,7 +6778,7 @@
         <v>93</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>1318</v>
+        <v>1310</v>
       </c>
       <c r="U14" s="3">
         <v>1125</v>
@@ -6786,7 +6787,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="24.95" customHeight="1">
       <c r="B15" t="s">
         <v>94</v>
       </c>
@@ -6809,7 +6810,7 @@
         <v>96</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>1305</v>
+        <v>1297</v>
       </c>
       <c r="M15" s="3">
         <v>1204</v>
@@ -6821,7 +6822,7 @@
         <v>53</v>
       </c>
       <c r="P15" s="40" t="s">
-        <v>1242</v>
+        <v>1234</v>
       </c>
       <c r="Q15" t="s">
         <v>97</v>
@@ -6833,7 +6834,7 @@
         <v>99</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>1319</v>
+        <v>1311</v>
       </c>
       <c r="U15" s="3">
         <v>1200</v>
@@ -6842,7 +6843,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="24.95" customHeight="1">
       <c r="B16" t="s">
         <v>101</v>
       </c>
@@ -6865,7 +6866,7 @@
         <v>33</v>
       </c>
       <c r="P16" s="40" t="s">
-        <v>1244</v>
+        <v>1236</v>
       </c>
       <c r="Q16" t="s">
         <v>103</v>
@@ -6883,7 +6884,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="17" spans="1:22" s="4" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" s="4" customFormat="1" ht="24.95" customHeight="1">
       <c r="A17" s="4" t="s">
         <v>107</v>
       </c>
@@ -6922,7 +6923,7 @@
         <v>33</v>
       </c>
       <c r="P17" s="41" t="s">
-        <v>1245</v>
+        <v>1237</v>
       </c>
       <c r="Q17" s="4" t="s">
         <v>111</v>
@@ -6940,7 +6941,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" ht="24.95" customHeight="1">
       <c r="A18" t="s">
         <v>114</v>
       </c>
@@ -6969,7 +6970,7 @@
         <v>33</v>
       </c>
       <c r="P18" s="40" t="s">
-        <v>1246</v>
+        <v>1238</v>
       </c>
       <c r="Q18" t="s">
         <v>116</v>
@@ -6987,7 +6988,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="19" spans="1:22" s="4" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" s="4" customFormat="1" ht="24.95" customHeight="1">
       <c r="B19" s="4" t="s">
         <v>119</v>
       </c>
@@ -7020,7 +7021,7 @@
         <v>53</v>
       </c>
       <c r="P19" s="41" t="s">
-        <v>1247</v>
+        <v>1239</v>
       </c>
       <c r="Q19" s="4" t="s">
         <v>123</v>
@@ -7038,7 +7039,7 @@
         <v>1346</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" ht="24.95" customHeight="1">
       <c r="A20" t="s">
         <v>126</v>
       </c>
@@ -7082,7 +7083,7 @@
         <v>33</v>
       </c>
       <c r="P20" s="40" t="s">
-        <v>1248</v>
+        <v>1240</v>
       </c>
       <c r="Q20" t="s">
         <v>129</v>
@@ -7103,7 +7104,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:22" s="4" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" s="4" customFormat="1" ht="24.95" customHeight="1">
       <c r="B21" s="4" t="s">
         <v>132</v>
       </c>
@@ -7131,7 +7132,7 @@
         <v>33</v>
       </c>
       <c r="P21" s="41" t="s">
-        <v>1249</v>
+        <v>1241</v>
       </c>
       <c r="Q21" s="4" t="s">
         <v>133</v>
@@ -7149,7 +7150,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" ht="24.95" customHeight="1">
       <c r="B22" t="s">
         <v>137</v>
       </c>
@@ -7172,7 +7173,7 @@
         <v>138</v>
       </c>
       <c r="O22" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P22" s="40" t="s">
         <v>755</v>
@@ -7193,7 +7194,7 @@
         <v>1568</v>
       </c>
     </row>
-    <row r="23" spans="1:22" s="4" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" s="4" customFormat="1" ht="24.95" customHeight="1">
       <c r="A23" s="4" t="s">
         <v>142</v>
       </c>
@@ -7232,7 +7233,7 @@
         <v>33</v>
       </c>
       <c r="P23" s="41" t="s">
-        <v>1250</v>
+        <v>1242</v>
       </c>
       <c r="Q23" s="4" t="s">
         <v>23</v>
@@ -7253,7 +7254,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" ht="24.95" customHeight="1">
       <c r="B24" t="s">
         <v>149</v>
       </c>
@@ -7282,10 +7283,10 @@
         <v>26</v>
       </c>
       <c r="O24" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P24" s="40" t="s">
-        <v>1251</v>
+        <v>1243</v>
       </c>
       <c r="Q24" t="s">
         <v>150</v>
@@ -7303,7 +7304,7 @@
         <v>1622</v>
       </c>
     </row>
-    <row r="25" spans="1:22" s="4" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" s="4" customFormat="1" ht="24.95" customHeight="1">
       <c r="B25" s="4" t="s">
         <v>153</v>
       </c>
@@ -7331,7 +7332,7 @@
         <v>53</v>
       </c>
       <c r="P25" s="41" t="s">
-        <v>1252</v>
+        <v>1244</v>
       </c>
       <c r="Q25" s="4" t="s">
         <v>154</v>
@@ -7352,7 +7353,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" ht="24.95" customHeight="1">
       <c r="B26" t="s">
         <v>157</v>
       </c>
@@ -7375,10 +7376,10 @@
         <v>158</v>
       </c>
       <c r="O26" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P26" s="40" t="s">
-        <v>1253</v>
+        <v>1245</v>
       </c>
       <c r="R26" s="2" t="s">
         <v>159</v>
@@ -7396,7 +7397,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" ht="24.95" customHeight="1">
       <c r="B27" t="s">
         <v>161</v>
       </c>
@@ -7431,7 +7432,7 @@
         <v>33</v>
       </c>
       <c r="P27" s="40" t="s">
-        <v>1254</v>
+        <v>1246</v>
       </c>
       <c r="Q27" t="s">
         <v>165</v>
@@ -7452,7 +7453,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" ht="24.95" customHeight="1">
       <c r="A28" t="s">
         <v>169</v>
       </c>
@@ -7481,7 +7482,7 @@
         <v>171</v>
       </c>
       <c r="O28" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P28" s="40" t="s">
         <v>736</v>
@@ -7505,7 +7506,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" ht="24.95" customHeight="1">
       <c r="A29" t="s">
         <v>175</v>
       </c>
@@ -7534,7 +7535,7 @@
         <v>1072</v>
       </c>
       <c r="M29" s="27" t="s">
-        <v>1428</v>
+        <v>1416</v>
       </c>
       <c r="N29" t="s">
         <v>39</v>
@@ -7543,7 +7544,7 @@
         <v>33</v>
       </c>
       <c r="P29" s="40" t="s">
-        <v>1255</v>
+        <v>1247</v>
       </c>
       <c r="Q29" t="s">
         <v>179</v>
@@ -7564,7 +7565,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" ht="24.95" customHeight="1">
       <c r="A30" t="s">
         <v>183</v>
       </c>
@@ -7587,22 +7588,22 @@
         <v>1074</v>
       </c>
       <c r="M30" s="27" t="s">
-        <v>1427</v>
+        <v>1415</v>
       </c>
       <c r="N30" t="s">
         <v>171</v>
       </c>
       <c r="O30" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P30" s="40" t="s">
-        <v>1256</v>
+        <v>1248</v>
       </c>
       <c r="Q30" t="s">
         <v>185</v>
       </c>
       <c r="R30" s="2" t="s">
-        <v>1360</v>
+        <v>1348</v>
       </c>
       <c r="S30" s="1" t="s">
         <v>186</v>
@@ -7611,10 +7612,10 @@
         <v>1139</v>
       </c>
       <c r="U30" s="27" t="s">
-        <v>1402</v>
+        <v>1390</v>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" ht="24.95" customHeight="1">
       <c r="A31" t="s">
         <v>187</v>
       </c>
@@ -7622,7 +7623,7 @@
         <v>188</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>1429</v>
+        <v>1417</v>
       </c>
       <c r="E31" t="s">
         <v>423</v>
@@ -7637,7 +7638,7 @@
         <v>1074</v>
       </c>
       <c r="M31" s="27" t="s">
-        <v>1426</v>
+        <v>1414</v>
       </c>
       <c r="N31" t="s">
         <v>53</v>
@@ -7646,7 +7647,7 @@
         <v>53</v>
       </c>
       <c r="P31" s="40" t="s">
-        <v>1257</v>
+        <v>1249</v>
       </c>
       <c r="Q31" t="s">
         <v>56</v>
@@ -7661,13 +7662,13 @@
         <v>192</v>
       </c>
       <c r="U31" s="27" t="s">
-        <v>1401</v>
+        <v>1389</v>
       </c>
       <c r="V31" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="32" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" ht="24.95" customHeight="1">
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="s">
         <v>193</v>
@@ -7706,7 +7707,7 @@
         <v>33</v>
       </c>
       <c r="P32" s="41" t="s">
-        <v>1258</v>
+        <v>1250</v>
       </c>
       <c r="Q32" s="4" t="s">
         <v>197</v>
@@ -7727,7 +7728,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="33" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" ht="24.95" customHeight="1">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
         <v>200</v>
@@ -7758,7 +7759,7 @@
         <v>33</v>
       </c>
       <c r="P33" s="41" t="s">
-        <v>1259</v>
+        <v>1251</v>
       </c>
       <c r="Q33" s="4" t="s">
         <v>197</v>
@@ -7779,7 +7780,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="34" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" ht="24.95" customHeight="1">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
         <v>203</v>
@@ -7812,7 +7813,7 @@
         <v>33</v>
       </c>
       <c r="P34" s="41" t="s">
-        <v>1260</v>
+        <v>1252</v>
       </c>
       <c r="Q34" s="4" t="s">
         <v>204</v>
@@ -7833,7 +7834,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="35" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" ht="24.95" customHeight="1">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
         <v>207</v>
@@ -7863,10 +7864,10 @@
         <v>73</v>
       </c>
       <c r="O35" s="4" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P35" s="41" t="s">
-        <v>1261</v>
+        <v>1253</v>
       </c>
       <c r="Q35" s="4" t="s">
         <v>73</v>
@@ -7887,7 +7888,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" ht="24.95" customHeight="1">
       <c r="A36" s="4"/>
       <c r="B36" s="4" t="s">
         <v>210</v>
@@ -7918,7 +7919,7 @@
         <v>33</v>
       </c>
       <c r="P36" s="41" t="s">
-        <v>1262</v>
+        <v>1254</v>
       </c>
       <c r="Q36" s="4" t="s">
         <v>211</v>
@@ -7939,7 +7940,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="37" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" ht="24.95" customHeight="1">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="s">
         <v>214</v>
@@ -7974,7 +7975,7 @@
         <v>33</v>
       </c>
       <c r="P37" s="41" t="s">
-        <v>1263</v>
+        <v>1255</v>
       </c>
       <c r="Q37" s="4" t="s">
         <v>23</v>
@@ -7995,7 +7996,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="38" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" ht="24.95" customHeight="1">
       <c r="A38" s="4"/>
       <c r="B38" s="4" t="s">
         <v>217</v>
@@ -8055,7 +8056,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="39" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" ht="24.95" customHeight="1">
       <c r="A39" s="4"/>
       <c r="B39" s="4" t="s">
         <v>222</v>
@@ -8086,7 +8087,7 @@
         <v>33</v>
       </c>
       <c r="P39" s="41" t="s">
-        <v>1264</v>
+        <v>1256</v>
       </c>
       <c r="Q39" s="5" t="s">
         <v>103</v>
@@ -8107,7 +8108,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" ht="24.95" customHeight="1">
       <c r="A40" s="4"/>
       <c r="B40" s="4" t="s">
         <v>226</v>
@@ -8138,7 +8139,7 @@
         <v>33</v>
       </c>
       <c r="P40" s="41" t="s">
-        <v>1246</v>
+        <v>1238</v>
       </c>
       <c r="Q40" s="4" t="s">
         <v>228</v>
@@ -8159,7 +8160,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" ht="24.95" customHeight="1">
       <c r="A41" s="4"/>
       <c r="B41" s="4" t="s">
         <v>231</v>
@@ -8190,7 +8191,7 @@
         <v>33</v>
       </c>
       <c r="P41" s="41" t="s">
-        <v>1265</v>
+        <v>1257</v>
       </c>
       <c r="Q41" s="4" t="s">
         <v>232</v>
@@ -8211,7 +8212,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" ht="24.95" customHeight="1">
       <c r="A42" s="4"/>
       <c r="B42" s="4" t="s">
         <v>235</v>
@@ -8250,7 +8251,7 @@
         <v>53</v>
       </c>
       <c r="P42" s="41" t="s">
-        <v>1266</v>
+        <v>1258</v>
       </c>
       <c r="Q42" s="4" t="s">
         <v>236</v>
@@ -8271,7 +8272,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" ht="24.95" customHeight="1">
       <c r="A43" s="4"/>
       <c r="B43" s="4" t="s">
         <v>239</v>
@@ -8310,7 +8311,7 @@
         <v>33</v>
       </c>
       <c r="P43" s="41" t="s">
-        <v>1255</v>
+        <v>1247</v>
       </c>
       <c r="Q43" s="4" t="s">
         <v>211</v>
@@ -8331,7 +8332,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="44" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" ht="24.95" customHeight="1">
       <c r="A44" s="4"/>
       <c r="B44" s="4" t="s">
         <v>242</v>
@@ -8366,7 +8367,7 @@
         <v>33</v>
       </c>
       <c r="P44" s="41" t="s">
-        <v>1267</v>
+        <v>1259</v>
       </c>
       <c r="Q44" s="5" t="s">
         <v>204</v>
@@ -8387,7 +8388,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" ht="24.95" customHeight="1">
       <c r="A45" s="4"/>
       <c r="B45" s="4" t="s">
         <v>245</v>
@@ -8420,7 +8421,7 @@
         <v>53</v>
       </c>
       <c r="P45" s="41" t="s">
-        <v>1244</v>
+        <v>1236</v>
       </c>
       <c r="Q45" s="4" t="s">
         <v>248</v>
@@ -8441,7 +8442,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="46" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" ht="24.95" customHeight="1">
       <c r="A46" s="4"/>
       <c r="B46" s="4" t="s">
         <v>251</v>
@@ -8477,10 +8478,10 @@
         <v>252</v>
       </c>
       <c r="O46" s="4" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P46" s="41" t="s">
-        <v>1268</v>
+        <v>1260</v>
       </c>
       <c r="Q46" s="4" t="s">
         <v>253</v>
@@ -8501,7 +8502,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="47" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" ht="24.95" customHeight="1">
       <c r="A47" s="4" t="s">
         <v>256</v>
       </c>
@@ -8531,10 +8532,10 @@
         <v>258</v>
       </c>
       <c r="O47" s="4" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P47" s="41" t="s">
-        <v>1269</v>
+        <v>1261</v>
       </c>
       <c r="Q47" s="4" t="s">
         <v>259</v>
@@ -8555,7 +8556,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="48" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" ht="24.95" customHeight="1">
       <c r="A48" s="4" t="s">
         <v>262</v>
       </c>
@@ -8590,7 +8591,7 @@
         <v>53</v>
       </c>
       <c r="P48" s="41" t="s">
-        <v>1270</v>
+        <v>1262</v>
       </c>
       <c r="Q48" s="4" t="s">
         <v>264</v>
@@ -8611,7 +8612,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="49" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" ht="24.95" customHeight="1">
       <c r="A49" s="4"/>
       <c r="B49" s="4" t="s">
         <v>267</v>
@@ -8652,7 +8653,7 @@
         <v>33</v>
       </c>
       <c r="P49" s="41" t="s">
-        <v>1271</v>
+        <v>1263</v>
       </c>
       <c r="Q49" s="4" t="s">
         <v>270</v>
@@ -8673,7 +8674,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" ht="24.95" customHeight="1">
       <c r="A50" s="4"/>
       <c r="B50" s="4" t="s">
         <v>273</v>
@@ -8697,10 +8698,10 @@
         <v>274</v>
       </c>
       <c r="O50" s="4" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P50" s="41" t="s">
-        <v>1265</v>
+        <v>1257</v>
       </c>
       <c r="Q50" s="4" t="s">
         <v>150</v>
@@ -8721,7 +8722,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="51" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" ht="24.95" customHeight="1">
       <c r="A51" s="4" t="s">
         <v>277</v>
       </c>
@@ -8775,7 +8776,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="52" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" ht="24.95" customHeight="1">
       <c r="A52" s="4"/>
       <c r="B52" s="4" t="s">
         <v>283</v>
@@ -8803,10 +8804,10 @@
         <v>284</v>
       </c>
       <c r="O52" s="4" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P52" s="41" t="s">
-        <v>1272</v>
+        <v>1264</v>
       </c>
       <c r="Q52" s="4" t="s">
         <v>285</v>
@@ -8827,7 +8828,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="53" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" ht="24.95" customHeight="1">
       <c r="A53" s="4" t="s">
         <v>288</v>
       </c>
@@ -8855,16 +8856,16 @@
       <c r="K53" s="4"/>
       <c r="L53" s="7"/>
       <c r="M53" s="10" t="s">
-        <v>1425</v>
+        <v>1413</v>
       </c>
       <c r="N53" s="4" t="s">
         <v>138</v>
       </c>
       <c r="O53" s="4" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P53" s="41" t="s">
-        <v>1273</v>
+        <v>1265</v>
       </c>
       <c r="Q53" s="4" t="s">
         <v>290</v>
@@ -8885,7 +8886,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="54" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" ht="24.95" customHeight="1">
       <c r="A54" s="4"/>
       <c r="B54" s="4" t="s">
         <v>293</v>
@@ -8913,10 +8914,10 @@
         <v>26</v>
       </c>
       <c r="O54" s="4" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P54" s="41" t="s">
-        <v>1274</v>
+        <v>1266</v>
       </c>
       <c r="Q54" s="4" t="s">
         <v>297</v>
@@ -8937,7 +8938,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="55" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" ht="24.95" customHeight="1">
       <c r="A55" s="4"/>
       <c r="B55" s="4" t="s">
         <v>296</v>
@@ -8965,10 +8966,10 @@
         <v>284</v>
       </c>
       <c r="O55" s="4" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P55" s="41" t="s">
-        <v>1275</v>
+        <v>1267</v>
       </c>
       <c r="Q55" s="4" t="s">
         <v>298</v>
@@ -8989,7 +8990,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="56" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" ht="24.95" customHeight="1">
       <c r="A56" s="4" t="s">
         <v>301</v>
       </c>
@@ -9019,16 +9020,16 @@
         <v>374</v>
       </c>
       <c r="M56" s="10" t="s">
-        <v>1424</v>
+        <v>1412</v>
       </c>
       <c r="N56" s="4" t="s">
         <v>171</v>
       </c>
       <c r="O56" s="4" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P56" s="41" t="s">
-        <v>1276</v>
+        <v>1268</v>
       </c>
       <c r="Q56" s="4" t="s">
         <v>303</v>
@@ -9049,7 +9050,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" ht="24.95" customHeight="1">
       <c r="A57" s="4"/>
       <c r="B57" s="4" t="s">
         <v>306</v>
@@ -9079,7 +9080,7 @@
         <v>26</v>
       </c>
       <c r="O57" s="4" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P57" s="41" t="s">
         <v>622</v>
@@ -9103,7 +9104,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="58" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" ht="24.95" customHeight="1">
       <c r="A58" s="4"/>
       <c r="B58" s="4" t="s">
         <v>310</v>
@@ -9131,7 +9132,7 @@
       <c r="K58" s="4"/>
       <c r="L58" s="7"/>
       <c r="M58" s="10" t="s">
-        <v>1423</v>
+        <v>1411</v>
       </c>
       <c r="N58" s="4" t="s">
         <v>53</v>
@@ -9140,7 +9141,7 @@
         <v>53</v>
       </c>
       <c r="P58" s="41" t="s">
-        <v>1277</v>
+        <v>1269</v>
       </c>
       <c r="Q58" s="4" t="s">
         <v>311</v>
@@ -9161,7 +9162,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="59" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" ht="24.95" customHeight="1">
       <c r="A59" s="7"/>
       <c r="B59" s="7" t="s">
         <v>314</v>
@@ -9194,7 +9195,7 @@
         <v>33</v>
       </c>
       <c r="P59" s="41" t="s">
-        <v>1278</v>
+        <v>1270</v>
       </c>
       <c r="Q59" s="7"/>
       <c r="R59" s="11" t="s">
@@ -9213,7 +9214,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="60" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" ht="24.95" customHeight="1">
       <c r="A60" s="4" t="s">
         <v>388</v>
       </c>
@@ -9271,11 +9272,11 @@
         <v>1168</v>
       </c>
       <c r="U60" s="10" t="s">
-        <v>1400</v>
+        <v>1388</v>
       </c>
       <c r="V60" s="4"/>
     </row>
-    <row r="61" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" ht="24.95" customHeight="1">
       <c r="A61" s="4" t="s">
         <v>322</v>
       </c>
@@ -9311,7 +9312,7 @@
         <v>1956</v>
       </c>
       <c r="M61" s="10" t="s">
-        <v>1422</v>
+        <v>1410</v>
       </c>
       <c r="N61" s="4" t="s">
         <v>39</v>
@@ -9320,7 +9321,7 @@
         <v>33</v>
       </c>
       <c r="P61" s="41" t="s">
-        <v>1279</v>
+        <v>1271</v>
       </c>
       <c r="Q61" s="4" t="s">
         <v>204</v>
@@ -9335,13 +9336,13 @@
         <v>1169</v>
       </c>
       <c r="U61" s="10" t="s">
-        <v>1399</v>
+        <v>1387</v>
       </c>
       <c r="V61" s="4" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="62" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" ht="24.95" customHeight="1">
       <c r="A62" t="s">
         <v>512</v>
       </c>
@@ -9367,7 +9368,7 @@
         <v>171</v>
       </c>
       <c r="O62" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P62" s="40" t="s">
         <v>516</v>
@@ -9382,16 +9383,16 @@
         <v>518</v>
       </c>
       <c r="T62" s="1" t="s">
-        <v>1170</v>
+        <v>1456</v>
       </c>
       <c r="U62" s="27" t="s">
-        <v>1396</v>
+        <v>1384</v>
       </c>
       <c r="V62" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="63" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" ht="24.95" customHeight="1">
       <c r="A63" t="s">
         <v>519</v>
       </c>
@@ -9417,7 +9418,7 @@
         <v>171</v>
       </c>
       <c r="O63" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P63" s="40" t="s">
         <v>522</v>
@@ -9432,13 +9433,13 @@
         <v>524</v>
       </c>
       <c r="T63" s="1" t="s">
-        <v>1171</v>
+        <v>1457</v>
       </c>
       <c r="U63" s="27" t="s">
-        <v>1398</v>
+        <v>1386</v>
       </c>
     </row>
-    <row r="64" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" ht="24.95" customHeight="1">
       <c r="A64" t="s">
         <v>525</v>
       </c>
@@ -9488,13 +9489,13 @@
         <v>536</v>
       </c>
       <c r="T64" s="1" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="U64" s="27" t="s">
-        <v>1397</v>
+        <v>1385</v>
       </c>
     </row>
-    <row r="65" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" ht="24.95" customHeight="1">
       <c r="A65" t="s">
         <v>537</v>
       </c>
@@ -9523,7 +9524,7 @@
         <v>171</v>
       </c>
       <c r="O65" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P65" s="40" t="s">
         <v>541</v>
@@ -9538,13 +9539,13 @@
         <v>543</v>
       </c>
       <c r="T65" s="1" t="s">
-        <v>1173</v>
+        <v>1458</v>
       </c>
       <c r="U65" s="27" t="s">
-        <v>1396</v>
+        <v>1384</v>
       </c>
     </row>
-    <row r="66" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22" ht="24.95" customHeight="1">
       <c r="A66" t="s">
         <v>544</v>
       </c>
@@ -9573,7 +9574,7 @@
         <v>26</v>
       </c>
       <c r="O66" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P66" s="40" t="s">
         <v>549</v>
@@ -9588,13 +9589,13 @@
         <v>552</v>
       </c>
       <c r="T66" s="1" t="s">
-        <v>1174</v>
+        <v>1459</v>
       </c>
       <c r="U66" s="3">
         <v>1935</v>
       </c>
     </row>
-    <row r="67" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" ht="24.95" customHeight="1">
       <c r="A67" t="s">
         <v>553</v>
       </c>
@@ -9638,7 +9639,7 @@
         <v>138</v>
       </c>
       <c r="O67" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P67" s="40" t="s">
         <v>549</v>
@@ -9653,13 +9654,13 @@
         <v>559</v>
       </c>
       <c r="T67" s="1" t="s">
-        <v>1175</v>
+        <v>1460</v>
       </c>
       <c r="U67" s="3">
         <v>1934</v>
       </c>
     </row>
-    <row r="68" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" ht="24.95" customHeight="1">
       <c r="A68" t="s">
         <v>560</v>
       </c>
@@ -9703,7 +9704,7 @@
         <v>138</v>
       </c>
       <c r="O68" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P68" s="40" t="s">
         <v>549</v>
@@ -9718,7 +9719,7 @@
         <v>567</v>
       </c>
       <c r="T68" s="1" t="s">
-        <v>1176</v>
+        <v>1461</v>
       </c>
       <c r="U68" s="3">
         <v>1918</v>
@@ -9727,7 +9728,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="69" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" ht="24.95" customHeight="1">
       <c r="A69" t="s">
         <v>569</v>
       </c>
@@ -9738,7 +9739,7 @@
         <v>430</v>
       </c>
       <c r="D69" s="27" t="s">
-        <v>1430</v>
+        <v>1418</v>
       </c>
       <c r="E69" t="s">
         <v>593</v>
@@ -9774,16 +9775,16 @@
         <v>573</v>
       </c>
       <c r="T69" s="1" t="s">
-        <v>1177</v>
+        <v>1171</v>
       </c>
       <c r="U69" s="27" t="s">
-        <v>1395</v>
+        <v>1383</v>
       </c>
       <c r="V69" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="70" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" ht="24.95" customHeight="1">
       <c r="A70" t="s">
         <v>575</v>
       </c>
@@ -9812,7 +9813,7 @@
         <v>171</v>
       </c>
       <c r="O70" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P70" s="40" t="s">
         <v>549</v>
@@ -9827,16 +9828,16 @@
         <v>579</v>
       </c>
       <c r="T70" s="1" t="s">
-        <v>1178</v>
+        <v>1172</v>
       </c>
       <c r="U70" s="27" t="s">
-        <v>1394</v>
+        <v>1382</v>
       </c>
       <c r="V70" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="71" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" ht="24.95" customHeight="1">
       <c r="A71" t="s">
         <v>581</v>
       </c>
@@ -9874,7 +9875,7 @@
         <v>171</v>
       </c>
       <c r="O71" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P71" s="40" t="s">
         <v>549</v>
@@ -9889,13 +9890,13 @@
         <v>585</v>
       </c>
       <c r="T71" s="1" t="s">
-        <v>1179</v>
+        <v>1173</v>
       </c>
       <c r="U71" s="27" t="s">
-        <v>1393</v>
+        <v>1381</v>
       </c>
     </row>
-    <row r="72" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22" ht="24.95" customHeight="1">
       <c r="A72" t="s">
         <v>586</v>
       </c>
@@ -9924,7 +9925,7 @@
         <v>171</v>
       </c>
       <c r="O72" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P72" s="40" t="s">
         <v>549</v>
@@ -9939,13 +9940,13 @@
         <v>590</v>
       </c>
       <c r="T72" s="1" t="s">
-        <v>1180</v>
+        <v>1462</v>
       </c>
       <c r="U72" s="27" t="s">
-        <v>1392</v>
+        <v>1380</v>
       </c>
     </row>
-    <row r="73" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" ht="24.95" customHeight="1">
       <c r="A73" t="s">
         <v>511</v>
       </c>
@@ -9998,7 +9999,7 @@
         <v>424</v>
       </c>
       <c r="T73" s="1" t="s">
-        <v>1181</v>
+        <v>1174</v>
       </c>
       <c r="U73" s="3" t="s">
         <v>1106</v>
@@ -10007,7 +10008,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="74" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" ht="24.95" customHeight="1">
       <c r="A74" t="s">
         <v>503</v>
       </c>
@@ -10045,16 +10046,16 @@
         <v>1902</v>
       </c>
       <c r="M74" s="27" t="s">
-        <v>1421</v>
+        <v>1409</v>
       </c>
       <c r="N74" t="s">
         <v>171</v>
       </c>
       <c r="O74" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P74" s="40" t="s">
-        <v>1280</v>
+        <v>1272</v>
       </c>
       <c r="Q74" t="s">
         <v>489</v>
@@ -10066,13 +10067,13 @@
         <v>424</v>
       </c>
       <c r="T74" s="1" t="s">
-        <v>1182</v>
+        <v>1175</v>
       </c>
       <c r="U74" s="27" t="s">
-        <v>1391</v>
+        <v>1379</v>
       </c>
     </row>
-    <row r="75" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" ht="24.95" customHeight="1">
       <c r="A75" t="s">
         <v>495</v>
       </c>
@@ -10116,7 +10117,7 @@
         <v>171</v>
       </c>
       <c r="O75" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P75" s="40" t="s">
         <v>490</v>
@@ -10131,13 +10132,13 @@
         <v>424</v>
       </c>
       <c r="T75" s="1" t="s">
-        <v>1183</v>
+        <v>1176</v>
       </c>
       <c r="U75" s="27" t="s">
-        <v>1390</v>
+        <v>1378</v>
       </c>
     </row>
-    <row r="76" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" ht="24.95" customHeight="1">
       <c r="A76" t="s">
         <v>487</v>
       </c>
@@ -10181,7 +10182,7 @@
         <v>171</v>
       </c>
       <c r="O76" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P76" s="40" t="s">
         <v>427</v>
@@ -10196,13 +10197,13 @@
         <v>424</v>
       </c>
       <c r="T76" s="1" t="s">
-        <v>1184</v>
+        <v>1177</v>
       </c>
       <c r="U76" s="27" t="s">
-        <v>1389</v>
+        <v>1377</v>
       </c>
     </row>
-    <row r="77" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" ht="24.95" customHeight="1">
       <c r="A77" t="s">
         <v>480</v>
       </c>
@@ -10246,7 +10247,7 @@
         <v>171</v>
       </c>
       <c r="O77" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P77" s="40" t="s">
         <v>474</v>
@@ -10261,16 +10262,16 @@
         <v>424</v>
       </c>
       <c r="T77" s="1" t="s">
-        <v>1185</v>
+        <v>1178</v>
       </c>
       <c r="U77" s="27" t="s">
-        <v>1388</v>
+        <v>1376</v>
       </c>
       <c r="V77" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="78" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22" ht="24.95" customHeight="1">
       <c r="A78" t="s">
         <v>470</v>
       </c>
@@ -10299,7 +10300,7 @@
         <v>171</v>
       </c>
       <c r="O78" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P78" s="40" t="s">
         <v>427</v>
@@ -10314,13 +10315,13 @@
         <v>424</v>
       </c>
       <c r="T78" s="1" t="s">
-        <v>1186</v>
+        <v>1179</v>
       </c>
       <c r="U78" s="27" t="s">
-        <v>1387</v>
+        <v>1375</v>
       </c>
     </row>
-    <row r="79" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22" ht="24.95" customHeight="1">
       <c r="A79" t="s">
         <v>467</v>
       </c>
@@ -10358,7 +10359,7 @@
         <v>171</v>
       </c>
       <c r="O79" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P79" s="40" t="s">
         <v>455</v>
@@ -10373,13 +10374,13 @@
         <v>424</v>
       </c>
       <c r="T79" s="1" t="s">
-        <v>1187</v>
+        <v>1180</v>
       </c>
       <c r="U79" s="27" t="s">
-        <v>1386</v>
+        <v>1374</v>
       </c>
     </row>
-    <row r="80" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" ht="24.95" customHeight="1">
       <c r="A80" t="s">
         <v>460</v>
       </c>
@@ -10414,7 +10415,7 @@
         <v>26</v>
       </c>
       <c r="O80" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P80" s="40" t="s">
         <v>455</v>
@@ -10429,13 +10430,13 @@
         <v>453</v>
       </c>
       <c r="T80" s="1" t="s">
-        <v>1188</v>
+        <v>1181</v>
       </c>
       <c r="U80" s="27" t="s">
-        <v>1385</v>
+        <v>1373</v>
       </c>
     </row>
-    <row r="81" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:22" ht="24.95" customHeight="1">
       <c r="A81" t="s">
         <v>452</v>
       </c>
@@ -10479,16 +10480,16 @@
         <v>444</v>
       </c>
       <c r="T81" s="1" t="s">
-        <v>1189</v>
+        <v>1182</v>
       </c>
       <c r="U81" s="27" t="s">
-        <v>1384</v>
+        <v>1372</v>
       </c>
       <c r="V81" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="82" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:22" ht="24.95" customHeight="1">
       <c r="A82" t="s">
         <v>442</v>
       </c>
@@ -10538,7 +10539,7 @@
         <v>434</v>
       </c>
       <c r="T82" s="1" t="s">
-        <v>1190</v>
+        <v>1183</v>
       </c>
       <c r="U82" s="3">
         <v>1900</v>
@@ -10547,7 +10548,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="83" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:22" ht="24.95" customHeight="1">
       <c r="A83" t="s">
         <v>432</v>
       </c>
@@ -10591,13 +10592,13 @@
         <v>424</v>
       </c>
       <c r="T83" s="1" t="s">
-        <v>1191</v>
+        <v>1184</v>
       </c>
       <c r="U83" s="3">
         <v>1925</v>
       </c>
     </row>
-    <row r="84" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:22" ht="24.95" customHeight="1">
       <c r="A84" s="4" t="s">
         <v>595</v>
       </c>
@@ -10608,7 +10609,7 @@
         <v>596</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>1316</v>
+        <v>1308</v>
       </c>
       <c r="E84" s="14" t="s">
         <v>597</v>
@@ -10631,7 +10632,7 @@
       <c r="K84" s="4"/>
       <c r="L84" s="7"/>
       <c r="M84" s="10" t="s">
-        <v>1420</v>
+        <v>1408</v>
       </c>
       <c r="N84" s="4" t="s">
         <v>53</v>
@@ -10652,7 +10653,7 @@
         <v>605</v>
       </c>
       <c r="T84" s="6" t="s">
-        <v>1192</v>
+        <v>1185</v>
       </c>
       <c r="U84" s="7" t="s">
         <v>606</v>
@@ -10661,7 +10662,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="85" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:22" ht="24.95" customHeight="1">
       <c r="A85" s="4" t="s">
         <v>607</v>
       </c>
@@ -10714,7 +10715,7 @@
         <v>615</v>
       </c>
       <c r="T85" s="6" t="s">
-        <v>1193</v>
+        <v>1186</v>
       </c>
       <c r="U85" s="7" t="s">
         <v>1107</v>
@@ -10723,7 +10724,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="86" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:22" ht="24.95" customHeight="1">
       <c r="A86" s="4"/>
       <c r="B86" s="4" t="s">
         <v>616</v>
@@ -10753,7 +10754,7 @@
       <c r="K86" s="4"/>
       <c r="L86" s="7"/>
       <c r="M86" s="10" t="s">
-        <v>1419</v>
+        <v>1407</v>
       </c>
       <c r="N86" s="4" t="s">
         <v>39</v>
@@ -10774,7 +10775,7 @@
         <v>624</v>
       </c>
       <c r="T86" s="4" t="s">
-        <v>1194</v>
+        <v>1187</v>
       </c>
       <c r="U86" s="7" t="s">
         <v>625</v>
@@ -10783,7 +10784,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="87" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:22" ht="24.95" customHeight="1">
       <c r="A87" s="4" t="s">
         <v>627</v>
       </c>
@@ -10813,7 +10814,7 @@
       <c r="K87" s="4"/>
       <c r="L87" s="7"/>
       <c r="M87" s="10" t="s">
-        <v>1418</v>
+        <v>1406</v>
       </c>
       <c r="N87" s="4" t="s">
         <v>53</v>
@@ -10834,7 +10835,7 @@
         <v>637</v>
       </c>
       <c r="T87" s="6" t="s">
-        <v>1195</v>
+        <v>1188</v>
       </c>
       <c r="U87" s="7" t="s">
         <v>638</v>
@@ -10843,7 +10844,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="88" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:22" ht="24.95" customHeight="1">
       <c r="A88" s="4" t="s">
         <v>640</v>
       </c>
@@ -10873,7 +10874,7 @@
       <c r="K88" s="4"/>
       <c r="L88" s="7"/>
       <c r="M88" s="10" t="s">
-        <v>1417</v>
+        <v>1405</v>
       </c>
       <c r="N88" s="4" t="s">
         <v>53</v>
@@ -10892,16 +10893,16 @@
         <v>649</v>
       </c>
       <c r="T88" s="6" t="s">
-        <v>1196</v>
+        <v>1189</v>
       </c>
       <c r="U88" s="10" t="s">
-        <v>1383</v>
+        <v>1371</v>
       </c>
       <c r="V88" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="89" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:22" ht="24.95" customHeight="1">
       <c r="A89" s="4" t="s">
         <v>650</v>
       </c>
@@ -10936,10 +10937,10 @@
         <v>656</v>
       </c>
       <c r="L89" s="7" t="s">
-        <v>1281</v>
+        <v>1273</v>
       </c>
       <c r="M89" s="10" t="s">
-        <v>1416</v>
+        <v>1404</v>
       </c>
       <c r="N89" s="4" t="s">
         <v>39</v>
@@ -10960,7 +10961,7 @@
         <v>659</v>
       </c>
       <c r="T89" s="6" t="s">
-        <v>1197</v>
+        <v>1190</v>
       </c>
       <c r="U89" s="7" t="s">
         <v>660</v>
@@ -10969,7 +10970,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="90" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:22" ht="24.95" customHeight="1">
       <c r="A90" s="4" t="s">
         <v>662</v>
       </c>
@@ -11007,7 +11008,7 @@
         <v>672</v>
       </c>
       <c r="M90" s="10" t="s">
-        <v>1415</v>
+        <v>1403</v>
       </c>
       <c r="N90" s="4" t="s">
         <v>39</v>
@@ -11028,16 +11029,16 @@
         <v>675</v>
       </c>
       <c r="T90" s="6" t="s">
-        <v>1198</v>
+        <v>1191</v>
       </c>
       <c r="U90" s="10" t="s">
-        <v>1382</v>
+        <v>1370</v>
       </c>
       <c r="V90" s="7" t="s">
         <v>671</v>
       </c>
     </row>
-    <row r="91" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:22" ht="24.95" customHeight="1">
       <c r="A91" s="4"/>
       <c r="B91" s="4" t="s">
         <v>676</v>
@@ -11065,7 +11066,7 @@
         <v>26</v>
       </c>
       <c r="O91" s="4" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P91" s="41" t="s">
         <v>679</v>
@@ -11078,14 +11079,14 @@
         <v>681</v>
       </c>
       <c r="T91" s="6" t="s">
-        <v>1199</v>
+        <v>1192</v>
       </c>
       <c r="U91" s="7" t="s">
         <v>1108</v>
       </c>
       <c r="V91" s="7"/>
     </row>
-    <row r="92" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:22" ht="24.95" customHeight="1">
       <c r="A92" s="4"/>
       <c r="B92" s="4" t="s">
         <v>682</v>
@@ -11131,7 +11132,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="93" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:22" ht="24.95" customHeight="1">
       <c r="A93" s="4"/>
       <c r="B93" s="4" t="s">
         <v>686</v>
@@ -11157,7 +11158,7 @@
         <v>26</v>
       </c>
       <c r="O93" s="4" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P93" s="41" t="s">
         <v>687</v>
@@ -11170,7 +11171,7 @@
         <v>689</v>
       </c>
       <c r="T93" s="6" t="s">
-        <v>1200</v>
+        <v>1193</v>
       </c>
       <c r="U93" s="7">
         <v>269</v>
@@ -11179,7 +11180,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:22" ht="24.95" customHeight="1">
       <c r="A94" s="4"/>
       <c r="B94" s="4" t="s">
         <v>690</v>
@@ -11207,7 +11208,7 @@
         <v>73</v>
       </c>
       <c r="O94" s="4" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P94" s="41" t="s">
         <v>691</v>
@@ -11220,7 +11221,7 @@
         <v>693</v>
       </c>
       <c r="T94" s="6" t="s">
-        <v>1201</v>
+        <v>1194</v>
       </c>
       <c r="U94" s="7">
         <v>304</v>
@@ -11229,7 +11230,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="95" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:22" ht="24.95" customHeight="1">
       <c r="A95" s="4" t="s">
         <v>694</v>
       </c>
@@ -11267,13 +11268,13 @@
         <v>1930</v>
       </c>
       <c r="M95" s="10" t="s">
-        <v>1414</v>
+        <v>1402</v>
       </c>
       <c r="N95" s="4" t="s">
         <v>701</v>
       </c>
       <c r="O95" s="4" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P95" s="41" t="s">
         <v>702</v>
@@ -11288,7 +11289,7 @@
         <v>705</v>
       </c>
       <c r="T95" s="6" t="s">
-        <v>1202</v>
+        <v>1195</v>
       </c>
       <c r="U95" s="7">
         <v>1937</v>
@@ -11297,7 +11298,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="96" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:22" ht="24.95" customHeight="1">
       <c r="A96" s="4"/>
       <c r="B96" s="4" t="s">
         <v>706</v>
@@ -11340,7 +11341,7 @@
         <v>713</v>
       </c>
       <c r="T96" s="33" t="s">
-        <v>1203</v>
+        <v>1196</v>
       </c>
       <c r="U96" s="7" t="s">
         <v>714</v>
@@ -11349,7 +11350,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="97" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:22" ht="24.95" customHeight="1">
       <c r="A97" s="4" t="s">
         <v>716</v>
       </c>
@@ -11389,7 +11390,7 @@
         <v>171</v>
       </c>
       <c r="O97" s="4" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P97" s="41" t="s">
         <v>722</v>
@@ -11404,14 +11405,14 @@
         <v>724</v>
       </c>
       <c r="T97" s="33" t="s">
-        <v>1204</v>
+        <v>1197</v>
       </c>
       <c r="U97" s="7">
         <v>1937</v>
       </c>
       <c r="V97" s="7"/>
     </row>
-    <row r="98" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:22" ht="24.95" customHeight="1">
       <c r="A98" s="4"/>
       <c r="B98" s="4" t="s">
         <v>725</v>
@@ -11437,7 +11438,7 @@
         <v>171</v>
       </c>
       <c r="O98" s="4" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P98" s="41" t="s">
         <v>727</v>
@@ -11459,7 +11460,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="99" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:22" ht="24.95" customHeight="1">
       <c r="A99" s="4"/>
       <c r="B99" s="4" t="s">
         <v>730</v>
@@ -11485,7 +11486,7 @@
         <v>26</v>
       </c>
       <c r="O99" s="4" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P99" s="41" t="s">
         <v>732</v>
@@ -11498,14 +11499,14 @@
         <v>734</v>
       </c>
       <c r="T99" s="6" t="s">
-        <v>1205</v>
+        <v>1198</v>
       </c>
       <c r="U99" s="7" t="s">
         <v>1065</v>
       </c>
       <c r="V99" s="7"/>
     </row>
-    <row r="100" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:22" ht="24.95" customHeight="1">
       <c r="A100" s="4"/>
       <c r="B100" s="4" t="s">
         <v>735</v>
@@ -11527,7 +11528,7 @@
         <v>26</v>
       </c>
       <c r="O100" s="4" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P100" s="41" t="s">
         <v>736</v>
@@ -11547,7 +11548,7 @@
       </c>
       <c r="V100" s="7"/>
     </row>
-    <row r="101" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:22" ht="24.95" customHeight="1">
       <c r="B101" t="s">
         <v>742</v>
       </c>
@@ -11558,7 +11559,7 @@
         <v>171</v>
       </c>
       <c r="O101" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P101" s="40" t="s">
         <v>743</v>
@@ -11579,7 +11580,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="102" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:22" ht="24.95" customHeight="1">
       <c r="B102" t="s">
         <v>746</v>
       </c>
@@ -11590,7 +11591,7 @@
         <v>171</v>
       </c>
       <c r="O102" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P102" s="40" t="s">
         <v>747</v>
@@ -11605,11 +11606,11 @@
         <v>749</v>
       </c>
       <c r="T102" s="1" t="s">
-        <v>1206</v>
+        <v>1199</v>
       </c>
       <c r="V102" s="3"/>
     </row>
-    <row r="103" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:22" ht="24.95" customHeight="1">
       <c r="B103" t="s">
         <v>750</v>
       </c>
@@ -11620,7 +11621,7 @@
         <v>171</v>
       </c>
       <c r="O103" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P103" s="40" t="s">
         <v>751</v>
@@ -11635,11 +11636,11 @@
         <v>753</v>
       </c>
       <c r="T103" s="1" t="s">
-        <v>1207</v>
+        <v>1200</v>
       </c>
       <c r="V103" s="3"/>
     </row>
-    <row r="104" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:22" ht="24.95" customHeight="1">
       <c r="B104" t="s">
         <v>754</v>
       </c>
@@ -11665,14 +11666,14 @@
         <v>757</v>
       </c>
       <c r="T104" s="1" t="s">
-        <v>1208</v>
+        <v>1201</v>
       </c>
       <c r="U104" s="3">
         <v>470</v>
       </c>
       <c r="V104" s="3"/>
     </row>
-    <row r="105" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:22" ht="24.95" customHeight="1">
       <c r="A105" s="18" t="s">
         <v>758</v>
       </c>
@@ -11700,7 +11701,7 @@
       <c r="K105" s="19"/>
       <c r="L105" s="25"/>
       <c r="M105" s="31" t="s">
-        <v>1412</v>
+        <v>1400</v>
       </c>
       <c r="N105" s="19" t="s">
         <v>532</v>
@@ -11709,7 +11710,7 @@
         <v>53</v>
       </c>
       <c r="P105" s="30" t="s">
-        <v>1282</v>
+        <v>1274</v>
       </c>
       <c r="Q105" s="19" t="s">
         <v>764</v>
@@ -11717,11 +11718,11 @@
       <c r="R105" s="19" t="s">
         <v>765</v>
       </c>
-      <c r="S105" s="19" t="s">
+      <c r="S105" s="32" t="s">
         <v>766</v>
       </c>
-      <c r="T105" s="19" t="s">
-        <v>1209</v>
+      <c r="T105" s="36" t="s">
+        <v>1463</v>
       </c>
       <c r="U105" s="25" t="s">
         <v>1109</v>
@@ -11730,7 +11731,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="106" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:22" ht="24.95" customHeight="1">
       <c r="A106" s="21" t="s">
         <v>768</v>
       </c>
@@ -11763,19 +11764,19 @@
         <v>773</v>
       </c>
       <c r="L106" s="26" t="s">
-        <v>1306</v>
+        <v>1298</v>
       </c>
       <c r="M106" s="24" t="s">
-        <v>1413</v>
+        <v>1401</v>
       </c>
       <c r="N106" s="22" t="s">
         <v>171</v>
       </c>
       <c r="O106" s="22" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P106" s="29" t="s">
-        <v>1283</v>
+        <v>1275</v>
       </c>
       <c r="Q106" s="22" t="s">
         <v>774</v>
@@ -11790,11 +11791,11 @@
         <v>777</v>
       </c>
       <c r="U106" s="24" t="s">
-        <v>1381</v>
+        <v>1369</v>
       </c>
       <c r="V106" s="23"/>
     </row>
-    <row r="107" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:22" ht="24.95" customHeight="1">
       <c r="A107" s="18"/>
       <c r="B107" s="19" t="s">
         <v>778</v>
@@ -11825,7 +11826,7 @@
         <v>53</v>
       </c>
       <c r="P107" s="30" t="s">
-        <v>1284</v>
+        <v>1276</v>
       </c>
       <c r="Q107" s="19" t="s">
         <v>781</v>
@@ -11834,17 +11835,17 @@
         <v>782</v>
       </c>
       <c r="S107" s="32" t="s">
-        <v>1320</v>
+        <v>1312</v>
       </c>
       <c r="T107" s="32" t="s">
-        <v>1210</v>
+        <v>1202</v>
       </c>
       <c r="U107" s="25" t="s">
         <v>1110</v>
       </c>
       <c r="V107" s="20"/>
     </row>
-    <row r="108" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:22" ht="24.95" customHeight="1">
       <c r="A108" s="21" t="s">
         <v>783</v>
       </c>
@@ -11888,10 +11889,10 @@
         <v>171</v>
       </c>
       <c r="O108" s="22" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P108" s="29" t="s">
-        <v>1285</v>
+        <v>1277</v>
       </c>
       <c r="Q108" s="22" t="s">
         <v>791</v>
@@ -11903,16 +11904,16 @@
         <v>793</v>
       </c>
       <c r="T108" s="34" t="s">
-        <v>1211</v>
+        <v>1203</v>
       </c>
       <c r="U108" s="24" t="s">
-        <v>1380</v>
+        <v>1368</v>
       </c>
       <c r="V108" s="23" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="109" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:22" ht="24.95" customHeight="1">
       <c r="A109" s="18" t="s">
         <v>794</v>
       </c>
@@ -11950,16 +11951,16 @@
         <v>801</v>
       </c>
       <c r="M109" s="31" t="s">
-        <v>1405</v>
+        <v>1393</v>
       </c>
       <c r="N109" s="19" t="s">
         <v>171</v>
       </c>
       <c r="O109" s="19" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P109" s="30" t="s">
-        <v>1286</v>
+        <v>1278</v>
       </c>
       <c r="Q109" s="19" t="s">
         <v>802</v>
@@ -11971,14 +11972,14 @@
         <v>804</v>
       </c>
       <c r="T109" s="32" t="s">
-        <v>1212</v>
+        <v>1204</v>
       </c>
       <c r="U109" s="31" t="s">
-        <v>1379</v>
+        <v>1367</v>
       </c>
       <c r="V109" s="20"/>
     </row>
-    <row r="110" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:22" ht="24.95" customHeight="1">
       <c r="A110" s="21" t="s">
         <v>805</v>
       </c>
@@ -12012,10 +12013,10 @@
         <v>258</v>
       </c>
       <c r="O110" s="35" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P110" s="29" t="s">
-        <v>1287</v>
+        <v>1279</v>
       </c>
       <c r="Q110" s="22" t="s">
         <v>810</v>
@@ -12027,7 +12028,7 @@
         <v>812</v>
       </c>
       <c r="T110" s="34" t="s">
-        <v>1213</v>
+        <v>1205</v>
       </c>
       <c r="U110" s="26" t="s">
         <v>1111</v>
@@ -12036,7 +12037,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="111" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:22" ht="24.95" customHeight="1">
       <c r="A111" s="18" t="s">
         <v>814</v>
       </c>
@@ -12069,19 +12070,19 @@
         <v>819</v>
       </c>
       <c r="L111" s="25" t="s">
-        <v>1307</v>
+        <v>1299</v>
       </c>
       <c r="M111" s="31" t="s">
-        <v>1412</v>
+        <v>1400</v>
       </c>
       <c r="N111" s="19" t="s">
         <v>171</v>
       </c>
       <c r="O111" s="19" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P111" s="30" t="s">
-        <v>1288</v>
+        <v>1280</v>
       </c>
       <c r="Q111" s="19" t="s">
         <v>774</v>
@@ -12093,16 +12094,16 @@
         <v>821</v>
       </c>
       <c r="T111" s="32" t="s">
-        <v>1214</v>
+        <v>1206</v>
       </c>
       <c r="U111" s="31" t="s">
-        <v>1378</v>
+        <v>1366</v>
       </c>
       <c r="V111" s="20" t="s">
         <v>822</v>
       </c>
     </row>
-    <row r="112" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:22" ht="24.95" customHeight="1">
       <c r="A112" s="21" t="s">
         <v>823</v>
       </c>
@@ -12140,16 +12141,16 @@
         <v>831</v>
       </c>
       <c r="M112" s="24" t="s">
-        <v>1411</v>
+        <v>1399</v>
       </c>
       <c r="N112" s="22" t="s">
         <v>171</v>
       </c>
       <c r="O112" s="22" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P112" s="29" t="s">
-        <v>1276</v>
+        <v>1268</v>
       </c>
       <c r="Q112" s="22" t="s">
         <v>802</v>
@@ -12161,16 +12162,16 @@
         <v>833</v>
       </c>
       <c r="T112" s="34" t="s">
-        <v>1215</v>
+        <v>1207</v>
       </c>
       <c r="U112" s="24" t="s">
-        <v>1377</v>
+        <v>1365</v>
       </c>
       <c r="V112" s="23" t="s">
         <v>678</v>
       </c>
     </row>
-    <row r="113" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:22" ht="24.95" customHeight="1">
       <c r="A113" s="18" t="s">
         <v>834</v>
       </c>
@@ -12208,10 +12209,10 @@
         <v>258</v>
       </c>
       <c r="O113" s="36" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P113" s="30" t="s">
-        <v>1287</v>
+        <v>1279</v>
       </c>
       <c r="Q113" s="19" t="s">
         <v>810</v>
@@ -12223,7 +12224,7 @@
         <v>840</v>
       </c>
       <c r="T113" s="32" t="s">
-        <v>1216</v>
+        <v>1208</v>
       </c>
       <c r="U113" s="25" t="s">
         <v>1111</v>
@@ -12232,7 +12233,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="114" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:22" ht="24.95" customHeight="1">
       <c r="A114" s="21" t="s">
         <v>841</v>
       </c>
@@ -12267,10 +12268,10 @@
         <v>847</v>
       </c>
       <c r="L114" s="26" t="s">
-        <v>1308</v>
+        <v>1300</v>
       </c>
       <c r="M114" s="24" t="s">
-        <v>1410</v>
+        <v>1398</v>
       </c>
       <c r="N114" s="22" t="s">
         <v>39</v>
@@ -12291,16 +12292,16 @@
         <v>851</v>
       </c>
       <c r="T114" s="34" t="s">
-        <v>1217</v>
+        <v>1209</v>
       </c>
       <c r="U114" s="24" t="s">
-        <v>1376</v>
+        <v>1364</v>
       </c>
       <c r="V114" s="23" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="115" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:22" ht="24.95" customHeight="1">
       <c r="A115" s="18" t="s">
         <v>852</v>
       </c>
@@ -12335,7 +12336,7 @@
         <v>33</v>
       </c>
       <c r="P115" s="30" t="s">
-        <v>1289</v>
+        <v>1281</v>
       </c>
       <c r="Q115" s="19" t="s">
         <v>856</v>
@@ -12347,7 +12348,7 @@
         <v>858</v>
       </c>
       <c r="T115" s="32" t="s">
-        <v>1218</v>
+        <v>1210</v>
       </c>
       <c r="U115" s="25" t="s">
         <v>1112</v>
@@ -12356,7 +12357,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="116" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:22" ht="24.95" customHeight="1">
       <c r="A116" s="21" t="s">
         <v>859</v>
       </c>
@@ -12383,21 +12384,21 @@
         <v>863</v>
       </c>
       <c r="J116" s="26" t="s">
-        <v>1315</v>
+        <v>1307</v>
       </c>
       <c r="K116" s="22"/>
       <c r="L116" s="26"/>
       <c r="M116" s="24" t="s">
-        <v>1409</v>
+        <v>1397</v>
       </c>
       <c r="N116" s="22" t="s">
         <v>171</v>
       </c>
       <c r="O116" s="35" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P116" s="29" t="s">
-        <v>1290</v>
+        <v>1282</v>
       </c>
       <c r="Q116" s="22" t="s">
         <v>774</v>
@@ -12409,16 +12410,16 @@
         <v>865</v>
       </c>
       <c r="T116" s="34" t="s">
-        <v>1219</v>
+        <v>1211</v>
       </c>
       <c r="U116" s="24" t="s">
-        <v>1375</v>
+        <v>1363</v>
       </c>
       <c r="V116" s="23" t="s">
         <v>866</v>
       </c>
     </row>
-    <row r="117" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:22" ht="24.95" customHeight="1">
       <c r="A117" s="18" t="s">
         <v>867</v>
       </c>
@@ -12452,16 +12453,16 @@
       <c r="K117" s="19"/>
       <c r="L117" s="25"/>
       <c r="M117" s="31" t="s">
-        <v>1408</v>
+        <v>1396</v>
       </c>
       <c r="N117" s="19" t="s">
         <v>138</v>
       </c>
       <c r="O117" s="19" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P117" s="30" t="s">
-        <v>1291</v>
+        <v>1283</v>
       </c>
       <c r="Q117" s="19" t="s">
         <v>873</v>
@@ -12473,14 +12474,14 @@
         <v>875</v>
       </c>
       <c r="T117" s="32" t="s">
-        <v>1220</v>
+        <v>1212</v>
       </c>
       <c r="U117" s="31" t="s">
-        <v>1374</v>
+        <v>1362</v>
       </c>
       <c r="V117" s="20"/>
     </row>
-    <row r="118" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:22" ht="24.95" customHeight="1">
       <c r="A118" s="21" t="s">
         <v>876</v>
       </c>
@@ -12510,10 +12511,10 @@
         <v>171</v>
       </c>
       <c r="O118" s="22" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P118" s="29" t="s">
-        <v>1292</v>
+        <v>1284</v>
       </c>
       <c r="Q118" s="22" t="s">
         <v>774</v>
@@ -12525,14 +12526,14 @@
         <v>879</v>
       </c>
       <c r="T118" s="34" t="s">
-        <v>1221</v>
+        <v>1213</v>
       </c>
       <c r="U118" s="24" t="s">
-        <v>1363</v>
+        <v>1351</v>
       </c>
       <c r="V118" s="23"/>
     </row>
-    <row r="119" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:22" ht="24.95" customHeight="1">
       <c r="A119" s="18" t="s">
         <v>880</v>
       </c>
@@ -12569,7 +12570,7 @@
         <v>53</v>
       </c>
       <c r="P119" s="30" t="s">
-        <v>1293</v>
+        <v>1285</v>
       </c>
       <c r="Q119" s="19" t="s">
         <v>781</v>
@@ -12578,7 +12579,7 @@
         <v>885</v>
       </c>
       <c r="S119" s="32" t="s">
-        <v>1321</v>
+        <v>1313</v>
       </c>
       <c r="T119" s="32" t="s">
         <v>886</v>
@@ -12590,7 +12591,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="120" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:22" ht="24.95" customHeight="1">
       <c r="A120" s="21" t="s">
         <v>888</v>
       </c>
@@ -12601,7 +12602,7 @@
         <v>889</v>
       </c>
       <c r="D120" s="24" t="s">
-        <v>1361</v>
+        <v>1349</v>
       </c>
       <c r="E120" s="22" t="s">
         <v>887</v>
@@ -12625,7 +12626,7 @@
         <v>354</v>
       </c>
       <c r="L120" s="26" t="s">
-        <v>1309</v>
+        <v>1301</v>
       </c>
       <c r="M120" s="29" t="s">
         <v>1097</v>
@@ -12634,7 +12635,7 @@
         <v>138</v>
       </c>
       <c r="O120" s="35" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P120" s="29" t="s">
         <v>893</v>
@@ -12652,11 +12653,11 @@
         <v>897</v>
       </c>
       <c r="U120" s="24" t="s">
-        <v>1373</v>
+        <v>1361</v>
       </c>
       <c r="V120" s="23"/>
     </row>
-    <row r="121" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:22" ht="24.95" customHeight="1">
       <c r="A121" s="18" t="s">
         <v>898</v>
       </c>
@@ -12689,16 +12690,16 @@
         <v>902</v>
       </c>
       <c r="L121" s="25" t="s">
-        <v>1310</v>
+        <v>1302</v>
       </c>
       <c r="M121" s="31" t="s">
-        <v>1407</v>
+        <v>1395</v>
       </c>
       <c r="N121" s="19" t="s">
         <v>171</v>
       </c>
       <c r="O121" s="19" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P121" s="30" t="s">
         <v>903</v>
@@ -12713,14 +12714,14 @@
         <v>905</v>
       </c>
       <c r="T121" s="32" t="s">
-        <v>1222</v>
+        <v>1214</v>
       </c>
       <c r="U121" s="31" t="s">
-        <v>1372</v>
+        <v>1360</v>
       </c>
       <c r="V121" s="20"/>
     </row>
-    <row r="122" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:22" ht="24.95" customHeight="1">
       <c r="A122" s="21" t="s">
         <v>906</v>
       </c>
@@ -12756,16 +12757,16 @@
         <v>911</v>
       </c>
       <c r="M122" s="24" t="s">
-        <v>1406</v>
+        <v>1394</v>
       </c>
       <c r="N122" s="22" t="s">
         <v>171</v>
       </c>
       <c r="O122" s="22" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P122" s="29" t="s">
-        <v>1294</v>
+        <v>1286</v>
       </c>
       <c r="Q122" s="22" t="s">
         <v>774</v>
@@ -12777,16 +12778,16 @@
         <v>913</v>
       </c>
       <c r="T122" s="34" t="s">
-        <v>1223</v>
+        <v>1215</v>
       </c>
       <c r="U122" s="24" t="s">
-        <v>1371</v>
+        <v>1359</v>
       </c>
       <c r="V122" s="23" t="s">
         <v>914</v>
       </c>
     </row>
-    <row r="123" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:22" ht="24.95" customHeight="1">
       <c r="A123" s="18" t="s">
         <v>915</v>
       </c>
@@ -12821,7 +12822,7 @@
         <v>354</v>
       </c>
       <c r="L123" s="25" t="s">
-        <v>1311</v>
+        <v>1303</v>
       </c>
       <c r="M123" s="30" t="s">
         <v>1096</v>
@@ -12833,7 +12834,7 @@
         <v>33</v>
       </c>
       <c r="P123" s="30" t="s">
-        <v>1295</v>
+        <v>1287</v>
       </c>
       <c r="Q123" s="19" t="s">
         <v>920</v>
@@ -12845,16 +12846,16 @@
         <v>922</v>
       </c>
       <c r="T123" s="32" t="s">
-        <v>1224</v>
+        <v>1216</v>
       </c>
       <c r="U123" s="31" t="s">
-        <v>1370</v>
+        <v>1358</v>
       </c>
       <c r="V123" s="20" t="s">
         <v>923</v>
       </c>
     </row>
-    <row r="124" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:22" ht="24.95" customHeight="1">
       <c r="A124" s="21" t="s">
         <v>924</v>
       </c>
@@ -12889,7 +12890,7 @@
         <v>918</v>
       </c>
       <c r="L124" s="26" t="s">
-        <v>1312</v>
+        <v>1304</v>
       </c>
       <c r="M124" s="26">
         <v>2000</v>
@@ -12901,7 +12902,7 @@
         <v>53</v>
       </c>
       <c r="P124" s="29" t="s">
-        <v>1296</v>
+        <v>1288</v>
       </c>
       <c r="Q124" s="22" t="s">
         <v>929</v>
@@ -12913,7 +12914,7 @@
         <v>931</v>
       </c>
       <c r="T124" s="34" t="s">
-        <v>1225</v>
+        <v>1217</v>
       </c>
       <c r="U124" s="26" t="s">
         <v>1113</v>
@@ -12922,7 +12923,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="125" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:22" ht="24.95" customHeight="1">
       <c r="A125" s="18"/>
       <c r="B125" s="19" t="s">
         <v>933</v>
@@ -12951,7 +12952,7 @@
         <v>53</v>
       </c>
       <c r="P125" s="30" t="s">
-        <v>1297</v>
+        <v>1289</v>
       </c>
       <c r="Q125" s="19" t="s">
         <v>781</v>
@@ -12960,7 +12961,7 @@
         <v>935</v>
       </c>
       <c r="S125" s="32" t="s">
-        <v>1322</v>
+        <v>1314</v>
       </c>
       <c r="T125" s="32" t="s">
         <v>936</v>
@@ -12972,7 +12973,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="126" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:22" ht="24.95" customHeight="1">
       <c r="A126" s="21" t="s">
         <v>880</v>
       </c>
@@ -13009,7 +13010,7 @@
         <v>53</v>
       </c>
       <c r="P126" s="29" t="s">
-        <v>1298</v>
+        <v>1290</v>
       </c>
       <c r="Q126" s="22" t="s">
         <v>781</v>
@@ -13018,7 +13019,7 @@
         <v>941</v>
       </c>
       <c r="S126" s="34" t="s">
-        <v>1321</v>
+        <v>1313</v>
       </c>
       <c r="T126" s="34" t="s">
         <v>886</v>
@@ -13030,7 +13031,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="127" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:22" ht="24.95" customHeight="1">
       <c r="A127" s="18" t="s">
         <v>943</v>
       </c>
@@ -13070,10 +13071,10 @@
         <v>171</v>
       </c>
       <c r="O127" s="19" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P127" s="30" t="s">
-        <v>1299</v>
+        <v>1291</v>
       </c>
       <c r="Q127" s="19" t="s">
         <v>802</v>
@@ -13085,16 +13086,16 @@
         <v>949</v>
       </c>
       <c r="T127" s="32" t="s">
-        <v>1226</v>
+        <v>1218</v>
       </c>
       <c r="U127" s="31" t="s">
-        <v>1369</v>
+        <v>1357</v>
       </c>
       <c r="V127" s="20" t="s">
         <v>950</v>
       </c>
     </row>
-    <row r="128" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:22" ht="24.95" customHeight="1">
       <c r="A128" s="18" t="s">
         <v>952</v>
       </c>
@@ -13126,16 +13127,16 @@
       <c r="K128" s="19"/>
       <c r="L128" s="25"/>
       <c r="M128" s="31" t="s">
-        <v>1405</v>
+        <v>1393</v>
       </c>
       <c r="N128" s="19" t="s">
         <v>171</v>
       </c>
       <c r="O128" s="19" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P128" s="30" t="s">
-        <v>1300</v>
+        <v>1292</v>
       </c>
       <c r="Q128" s="19" t="s">
         <v>774</v>
@@ -13147,14 +13148,14 @@
         <v>959</v>
       </c>
       <c r="T128" s="32" t="s">
-        <v>1227</v>
+        <v>1219</v>
       </c>
       <c r="U128" s="31" t="s">
-        <v>1368</v>
+        <v>1356</v>
       </c>
       <c r="V128" s="20"/>
     </row>
-    <row r="129" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:22" ht="24.95" customHeight="1">
       <c r="A129" s="21" t="s">
         <v>960</v>
       </c>
@@ -13192,16 +13193,16 @@
         <v>669</v>
       </c>
       <c r="M129" s="24" t="s">
-        <v>1404</v>
+        <v>1392</v>
       </c>
       <c r="N129" s="22" t="s">
         <v>171</v>
       </c>
       <c r="O129" s="22" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P129" s="29" t="s">
-        <v>1301</v>
+        <v>1293</v>
       </c>
       <c r="Q129" s="22" t="s">
         <v>802</v>
@@ -13213,14 +13214,14 @@
         <v>968</v>
       </c>
       <c r="T129" s="34" t="s">
-        <v>1228</v>
+        <v>1220</v>
       </c>
       <c r="U129" s="24" t="s">
-        <v>1367</v>
+        <v>1355</v>
       </c>
       <c r="V129" s="23"/>
     </row>
-    <row r="130" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:22" ht="24.95" customHeight="1">
       <c r="A130" s="18" t="s">
         <v>969</v>
       </c>
@@ -13253,7 +13254,7 @@
         <v>974</v>
       </c>
       <c r="L130" s="25" t="s">
-        <v>1313</v>
+        <v>1305</v>
       </c>
       <c r="M130" s="30" t="s">
         <v>1096</v>
@@ -13262,10 +13263,10 @@
         <v>171</v>
       </c>
       <c r="O130" s="19" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P130" s="30" t="s">
-        <v>1302</v>
+        <v>1294</v>
       </c>
       <c r="Q130" s="19" t="s">
         <v>774</v>
@@ -13280,11 +13281,11 @@
         <v>977</v>
       </c>
       <c r="U130" s="31" t="s">
-        <v>1363</v>
+        <v>1351</v>
       </c>
       <c r="V130" s="20"/>
     </row>
-    <row r="131" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:22" ht="24.95" customHeight="1">
       <c r="A131" s="21" t="s">
         <v>978</v>
       </c>
@@ -13320,10 +13321,10 @@
         <v>138</v>
       </c>
       <c r="O131" s="22" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P131" s="29" t="s">
-        <v>1302</v>
+        <v>1294</v>
       </c>
       <c r="Q131" s="22" t="s">
         <v>951</v>
@@ -13335,14 +13336,14 @@
         <v>984</v>
       </c>
       <c r="T131" s="34" t="s">
-        <v>1221</v>
+        <v>1213</v>
       </c>
       <c r="U131" s="24" t="s">
-        <v>1363</v>
+        <v>1351</v>
       </c>
       <c r="V131" s="23"/>
     </row>
-    <row r="132" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:22" ht="24.95" customHeight="1">
       <c r="A132" s="18" t="s">
         <v>985</v>
       </c>
@@ -13374,7 +13375,7 @@
       <c r="K132" s="19"/>
       <c r="L132" s="25"/>
       <c r="M132" s="31" t="s">
-        <v>1403</v>
+        <v>1391</v>
       </c>
       <c r="N132" s="19" t="s">
         <v>316</v>
@@ -13383,7 +13384,7 @@
         <v>33</v>
       </c>
       <c r="P132" s="30" t="s">
-        <v>1303</v>
+        <v>1295</v>
       </c>
       <c r="Q132" s="19" t="s">
         <v>991</v>
@@ -13395,7 +13396,7 @@
         <v>993</v>
       </c>
       <c r="T132" s="32" t="s">
-        <v>1229</v>
+        <v>1221</v>
       </c>
       <c r="U132" s="25" t="s">
         <v>1115</v>
@@ -13404,7 +13405,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="133" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:22" ht="24.95" customHeight="1">
       <c r="A133" s="21" t="s">
         <v>995</v>
       </c>
@@ -13439,7 +13440,7 @@
         <v>1001</v>
       </c>
       <c r="L133" s="26" t="s">
-        <v>1314</v>
+        <v>1306</v>
       </c>
       <c r="M133" s="29" t="s">
         <v>1096</v>
@@ -13448,10 +13449,10 @@
         <v>171</v>
       </c>
       <c r="O133" s="22" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P133" s="29" t="s">
-        <v>1302</v>
+        <v>1294</v>
       </c>
       <c r="Q133" s="22" t="s">
         <v>802</v>
@@ -13463,34 +13464,34 @@
         <v>1003</v>
       </c>
       <c r="T133" s="34" t="s">
-        <v>1230</v>
+        <v>1222</v>
       </c>
       <c r="U133" s="24" t="s">
-        <v>1363</v>
+        <v>1351</v>
       </c>
       <c r="V133" s="23"/>
     </row>
-    <row r="134" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:22" ht="24.95" customHeight="1">
       <c r="A134" s="42" t="s">
-        <v>1323</v>
+        <v>1315</v>
       </c>
       <c r="B134" s="43" t="s">
         <v>441</v>
       </c>
       <c r="C134" s="43" t="s">
-        <v>1327</v>
+        <v>1319</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>1324</v>
+        <v>1316</v>
       </c>
       <c r="E134" s="43" t="s">
-        <v>1325</v>
+        <v>1317</v>
       </c>
       <c r="F134" s="43" t="s">
         <v>483</v>
       </c>
       <c r="G134" s="43" t="s">
-        <v>1326</v>
+        <v>1318</v>
       </c>
       <c r="H134" s="3">
         <v>1940</v>
@@ -13502,45 +13503,45 @@
         <v>33</v>
       </c>
       <c r="O134" s="22" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P134" s="40" t="s">
-        <v>1335</v>
+        <v>1326</v>
       </c>
       <c r="Q134" s="43" t="s">
-        <v>1328</v>
+        <v>1320</v>
       </c>
       <c r="R134" s="43" t="s">
-        <v>1336</v>
-      </c>
-      <c r="T134" s="43" t="s">
-        <v>1329</v>
+        <v>1327</v>
+      </c>
+      <c r="T134" s="48" t="s">
+        <v>1465</v>
       </c>
       <c r="U134" s="27" t="s">
-        <v>1362</v>
+        <v>1350</v>
       </c>
       <c r="V134" s="43" t="s">
-        <v>1326</v>
+        <v>1318</v>
       </c>
     </row>
-    <row r="135" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:22" ht="24.95" customHeight="1">
       <c r="A135" s="44" t="s">
-        <v>1330</v>
+        <v>1321</v>
       </c>
       <c r="B135" s="45" t="s">
-        <v>1331</v>
+        <v>1322</v>
       </c>
       <c r="C135" s="45" t="s">
         <v>430</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>1332</v>
+        <v>1323</v>
       </c>
       <c r="E135" s="45" t="s">
-        <v>1333</v>
+        <v>1324</v>
       </c>
       <c r="F135" s="45" t="s">
-        <v>1334</v>
+        <v>1325</v>
       </c>
       <c r="G135" s="45" t="s">
         <v>354</v>
@@ -13555,51 +13556,51 @@
         <v>33</v>
       </c>
       <c r="O135" s="22" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="Q135" s="45" t="s">
         <v>802</v>
       </c>
       <c r="R135" s="45" t="s">
+        <v>1328</v>
+      </c>
+      <c r="S135" s="33" t="s">
+        <v>1329</v>
+      </c>
+      <c r="T135" s="33" t="s">
+        <v>1466</v>
+      </c>
+      <c r="U135" s="50" t="s">
+        <v>1352</v>
+      </c>
+      <c r="V135" t="s">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="136" spans="1:22" ht="24.95" customHeight="1">
+      <c r="A136" s="42" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B136" s="43" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C136" s="43" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="E136" s="43" t="s">
+        <v>1335</v>
+      </c>
+      <c r="F136" s="43" t="s">
+        <v>1336</v>
+      </c>
+      <c r="G136" s="47" t="s">
         <v>1337</v>
       </c>
-      <c r="S135" s="33" t="s">
-        <v>1338</v>
-      </c>
-      <c r="T135" s="33" t="s">
-        <v>1339</v>
-      </c>
-      <c r="U135" s="50" t="s">
-        <v>1364</v>
-      </c>
-      <c r="V135" t="s">
-        <v>1340</v>
-      </c>
-    </row>
-    <row r="136" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="42" t="s">
-        <v>1341</v>
-      </c>
-      <c r="B136" s="43" t="s">
-        <v>1342</v>
-      </c>
-      <c r="C136" s="43" t="s">
-        <v>1343</v>
-      </c>
-      <c r="D136" s="3" t="s">
-        <v>1344</v>
-      </c>
-      <c r="E136" s="43" t="s">
-        <v>1345</v>
-      </c>
-      <c r="F136" s="43" t="s">
-        <v>1346</v>
-      </c>
-      <c r="G136" s="47" t="s">
-        <v>1347</v>
-      </c>
       <c r="H136" s="27" t="s">
-        <v>1365</v>
+        <v>1353</v>
       </c>
       <c r="M136" s="3">
         <v>2000</v>
@@ -13608,33 +13609,33 @@
         <v>33</v>
       </c>
       <c r="O136" s="22" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P136" s="40" t="s">
-        <v>1359</v>
+        <v>1347</v>
       </c>
       <c r="Q136" s="43" t="s">
-        <v>1355</v>
+        <v>1344</v>
       </c>
       <c r="R136" s="43" t="s">
-        <v>1348</v>
-      </c>
-      <c r="S136" s="43" t="s">
-        <v>1349</v>
+        <v>1338</v>
+      </c>
+      <c r="S136" s="48" t="s">
+        <v>1339</v>
       </c>
       <c r="T136" s="48" t="s">
-        <v>1350</v>
+        <v>1464</v>
       </c>
       <c r="U136" s="27" t="s">
-        <v>1365</v>
+        <v>1353</v>
       </c>
       <c r="V136" s="43" t="s">
-        <v>1347</v>
+        <v>1337</v>
       </c>
     </row>
-    <row r="137" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:22" ht="24.95" customHeight="1">
       <c r="A137" s="44" t="s">
-        <v>1351</v>
+        <v>1340</v>
       </c>
       <c r="B137" s="45" t="s">
         <v>502</v>
@@ -13643,16 +13644,16 @@
         <v>509</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>1352</v>
+        <v>1341</v>
       </c>
       <c r="E137" s="45" t="s">
-        <v>1353</v>
+        <v>1342</v>
       </c>
       <c r="F137" s="45" t="s">
         <v>502</v>
       </c>
       <c r="G137" s="45" t="s">
-        <v>1354</v>
+        <v>1343</v>
       </c>
       <c r="H137" s="3">
         <v>1923</v>
@@ -13664,45 +13665,45 @@
         <v>33</v>
       </c>
       <c r="O137" s="22" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="Q137" s="45" t="s">
         <v>489</v>
       </c>
       <c r="R137" t="s">
-        <v>1357</v>
+        <v>1346</v>
       </c>
       <c r="S137" t="s">
-        <v>1356</v>
+        <v>1345</v>
       </c>
       <c r="T137" s="1" t="s">
-        <v>1358</v>
+        <v>1467</v>
       </c>
       <c r="U137" s="27" t="s">
-        <v>1366</v>
+        <v>1354</v>
       </c>
       <c r="V137" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="138" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:22" ht="24.95" customHeight="1">
       <c r="B138" s="51" t="s">
-        <v>1431</v>
+        <v>1419</v>
       </c>
       <c r="C138" s="51" t="s">
-        <v>1432</v>
+        <v>1420</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>1433</v>
+        <v>1421</v>
       </c>
       <c r="E138" s="51" t="s">
-        <v>1434</v>
+        <v>1422</v>
       </c>
       <c r="F138" s="51" t="s">
-        <v>1435</v>
+        <v>1423</v>
       </c>
       <c r="G138" s="43" t="s">
-        <v>1441</v>
+        <v>1429</v>
       </c>
       <c r="H138" s="3">
         <v>1330</v>
@@ -13717,42 +13718,42 @@
         <v>33</v>
       </c>
       <c r="P138" s="40" t="s">
-        <v>1436</v>
+        <v>1424</v>
       </c>
       <c r="Q138" s="51" t="s">
         <v>781</v>
       </c>
       <c r="R138" s="43" t="s">
-        <v>1442</v>
+        <v>1430</v>
       </c>
       <c r="S138" s="48" t="s">
-        <v>1437</v>
+        <v>1425</v>
       </c>
       <c r="T138" s="1" t="s">
-        <v>1438</v>
+        <v>1426</v>
       </c>
       <c r="U138" s="3" t="s">
-        <v>1439</v>
+        <v>1427</v>
       </c>
       <c r="V138" t="s">
-        <v>1440</v>
+        <v>1428</v>
       </c>
     </row>
-    <row r="139" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:22" ht="24.95" customHeight="1">
       <c r="B139" s="45" t="s">
-        <v>1443</v>
+        <v>1431</v>
       </c>
       <c r="C139" s="45" t="s">
         <v>430</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>1444</v>
+        <v>1432</v>
       </c>
       <c r="E139" s="45" t="s">
         <v>354</v>
       </c>
       <c r="G139" t="s">
-        <v>1450</v>
+        <v>1438</v>
       </c>
       <c r="H139" s="3">
         <v>1380</v>
@@ -13767,30 +13768,30 @@
         <v>33</v>
       </c>
       <c r="P139" s="40" t="s">
-        <v>1449</v>
+        <v>1437</v>
       </c>
       <c r="Q139" s="45" t="s">
         <v>85</v>
       </c>
       <c r="R139" s="45" t="s">
-        <v>1451</v>
+        <v>1439</v>
       </c>
       <c r="S139" s="1" t="s">
-        <v>1448</v>
+        <v>1436</v>
       </c>
       <c r="T139" s="1" t="s">
-        <v>1447</v>
+        <v>1435</v>
       </c>
       <c r="U139" s="3" t="s">
-        <v>1446</v>
+        <v>1434</v>
       </c>
       <c r="V139" t="s">
-        <v>1445</v>
+        <v>1433</v>
       </c>
     </row>
-    <row r="140" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:22" ht="24.95" customHeight="1">
       <c r="B140" s="51" t="s">
-        <v>1452</v>
+        <v>1440</v>
       </c>
       <c r="D140" s="3">
         <v>1329</v>
@@ -13799,7 +13800,7 @@
         <v>84</v>
       </c>
       <c r="G140" t="s">
-        <v>1453</v>
+        <v>1441</v>
       </c>
       <c r="H140" s="3">
         <v>1389</v>
@@ -13808,42 +13809,42 @@
         <v>26</v>
       </c>
       <c r="O140" s="45" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="P140" s="40" t="s">
-        <v>1454</v>
+        <v>1442</v>
       </c>
       <c r="Q140" s="51" t="s">
         <v>85</v>
       </c>
       <c r="R140" s="43" t="s">
-        <v>1455</v>
+        <v>1443</v>
       </c>
       <c r="S140" s="1" t="s">
-        <v>1459</v>
+        <v>1447</v>
       </c>
       <c r="T140" s="1" t="s">
-        <v>1458</v>
+        <v>1446</v>
       </c>
       <c r="U140" s="3" t="s">
-        <v>1457</v>
+        <v>1445</v>
       </c>
       <c r="V140" t="s">
-        <v>1456</v>
+        <v>1444</v>
       </c>
     </row>
-    <row r="141" spans="1:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B141" s="45" t="s">
-        <v>1460</v>
+    <row r="141" spans="1:22" ht="24.95" customHeight="1">
+      <c r="B141" s="52" t="s">
+        <v>1448</v>
       </c>
       <c r="C141" t="s">
-        <v>1461</v>
+        <v>1449</v>
       </c>
       <c r="D141" s="3">
         <v>1240</v>
       </c>
       <c r="E141" s="45" t="s">
-        <v>1462</v>
+        <v>1450</v>
       </c>
       <c r="G141" t="s">
         <v>506</v>
@@ -13861,25 +13862,25 @@
         <v>33</v>
       </c>
       <c r="P141" s="40" t="s">
-        <v>1463</v>
+        <v>1451</v>
       </c>
       <c r="Q141" s="45" t="s">
         <v>85</v>
       </c>
       <c r="R141" s="45" t="s">
-        <v>1467</v>
+        <v>1454</v>
       </c>
       <c r="S141" s="1" t="s">
-        <v>1466</v>
+        <v>1453</v>
       </c>
       <c r="T141" s="1" t="s">
-        <v>1465</v>
+        <v>1455</v>
       </c>
       <c r="U141" s="3">
         <v>1299</v>
       </c>
       <c r="V141" t="s">
-        <v>1464</v>
+        <v>1452</v>
       </c>
     </row>
   </sheetData>
@@ -14129,9 +14130,12 @@
     <hyperlink ref="S140" r:id="rId241"/>
     <hyperlink ref="T141" r:id="rId242"/>
     <hyperlink ref="S141" r:id="rId243"/>
+    <hyperlink ref="S105" r:id="rId244"/>
+    <hyperlink ref="S136" r:id="rId245"/>
+    <hyperlink ref="T134" r:id="rId246"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId244"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId247"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add state for url to person- and church- pages
</commit_message>
<xml_diff>
--- a/loadDatabase/religion/святые.xlsx
+++ b/loadDatabase/religion/святые.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12915" tabRatio="587"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18675" windowHeight="6675" tabRatio="587"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$W$140</definedName>
   </definedNames>
-  <calcPr calcId="124519" refMode="R1C1"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2173" uniqueCount="1467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2211" uniqueCount="1499">
   <si>
     <t>Фамилия</t>
   </si>
@@ -5512,6 +5512,102 @@
   </si>
   <si>
     <t>Святитель Пятирим</t>
+  </si>
+  <si>
+    <t>Ефрем Новоявленный Чудотворец</t>
+  </si>
+  <si>
+    <t>Священномученик Иаков Москаев</t>
+  </si>
+  <si>
+    <t>Священномученник Никита Прибытков</t>
+  </si>
+  <si>
+    <t>Преподобномученник Федор Никитин</t>
+  </si>
+  <si>
+    <t>Свещенномученик Петр Гаврилов</t>
+  </si>
+  <si>
+    <t>Священномученик Парфений (Брянский)</t>
+  </si>
+  <si>
+    <t>Священномученик Павел Гайдай</t>
+  </si>
+  <si>
+    <t>Священник Михаил Платонов</t>
+  </si>
+  <si>
+    <t>Священномученик Мирон Ржепик</t>
+  </si>
+  <si>
+    <t>Преподобномученник иеромонах Киприан</t>
+  </si>
+  <si>
+    <t>Священномученник Иоанн Мажорин</t>
+  </si>
+  <si>
+    <t>Преподобномученник ИОВ Протопопов</t>
+  </si>
+  <si>
+    <t>священник Иоанн Ганчев</t>
+  </si>
+  <si>
+    <t>Князь Георгий</t>
+  </si>
+  <si>
+    <t>Священномученник Георгий Садзаглишвили</t>
+  </si>
+  <si>
+    <t>Священномученик Владимир Пиксанов</t>
+  </si>
+  <si>
+    <t>Василий Ростовский</t>
+  </si>
+  <si>
+    <t>Священномученик Амросий Гудко</t>
+  </si>
+  <si>
+    <t>Священномученик Аркадий Остальский</t>
+  </si>
+  <si>
+    <t>Священномученик Александр Телемаков</t>
+  </si>
+  <si>
+    <t>Схимонахиня Августа Защук</t>
+  </si>
+  <si>
+    <t>Священномученик Августин Беляев</t>
+  </si>
+  <si>
+    <t>Мученик Александр Медем</t>
+  </si>
+  <si>
+    <t>Священномученник Нифонт Выблов</t>
+  </si>
+  <si>
+    <t>Священномученик Константин Сухов</t>
+  </si>
+  <si>
+    <t>Священномученник Алексий Орлов</t>
+  </si>
+  <si>
+    <t>Священномученик Александр Трапицын</t>
+  </si>
+  <si>
+    <t>Священномученник Анатолий Грисюк</t>
+  </si>
+  <si>
+    <t>Варсонофий Оптинский</t>
+  </si>
+  <si>
+    <t>Александр Чагринский</t>
+  </si>
+  <si>
+    <t>Сергий Радонежский</t>
+  </si>
+  <si>
+    <t>Серафим Саровский</t>
   </si>
 </sst>
 </file>
@@ -5619,7 +5715,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5640,6 +5736,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -5704,7 +5812,7 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5808,6 +5916,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -6094,8 +6207,8 @@
   <dimension ref="A1:W140"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E153" sqref="E153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8955,11 +9068,12 @@
       <c r="A53" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="B53" s="4"/>
+      <c r="B53" s="4" t="s">
+        <v>1467</v>
+      </c>
       <c r="C53" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D53" s="4"/>
       <c r="E53" s="7">
         <v>1384</v>
       </c>
@@ -10221,6 +10335,9 @@
       <c r="A75" t="s">
         <v>495</v>
       </c>
+      <c r="B75" t="s">
+        <v>1494</v>
+      </c>
       <c r="C75" t="s">
         <v>494</v>
       </c>
@@ -10286,6 +10403,9 @@
       <c r="A76" t="s">
         <v>487</v>
       </c>
+      <c r="B76" t="s">
+        <v>1493</v>
+      </c>
       <c r="C76" t="s">
         <v>486</v>
       </c>
@@ -10351,6 +10471,9 @@
       <c r="A77" t="s">
         <v>480</v>
       </c>
+      <c r="B77" t="s">
+        <v>1492</v>
+      </c>
       <c r="C77" t="s">
         <v>479</v>
       </c>
@@ -10419,6 +10542,9 @@
       <c r="A78" t="s">
         <v>470</v>
       </c>
+      <c r="B78" t="s">
+        <v>1491</v>
+      </c>
       <c r="C78" t="s">
         <v>161</v>
       </c>
@@ -10469,6 +10595,9 @@
       <c r="A79" t="s">
         <v>467</v>
       </c>
+      <c r="B79" t="s">
+        <v>1490</v>
+      </c>
       <c r="C79" t="s">
         <v>324</v>
       </c>
@@ -10528,6 +10657,9 @@
       <c r="A80" t="s">
         <v>460</v>
       </c>
+      <c r="B80" t="s">
+        <v>1489</v>
+      </c>
       <c r="C80" t="s">
         <v>459</v>
       </c>
@@ -10584,6 +10716,9 @@
       <c r="A81" t="s">
         <v>452</v>
       </c>
+      <c r="B81" t="s">
+        <v>1495</v>
+      </c>
       <c r="C81" t="s">
         <v>451</v>
       </c>
@@ -10636,6 +10771,9 @@
     <row r="82" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>442</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1496</v>
       </c>
       <c r="C82" t="s">
         <v>441</v>
@@ -10937,7 +11075,9 @@
       <c r="A87" s="4" t="s">
         <v>627</v>
       </c>
-      <c r="B87" s="4"/>
+      <c r="B87" s="4" t="s">
+        <v>1498</v>
+      </c>
       <c r="C87" s="4" t="s">
         <v>628</v>
       </c>
@@ -11401,7 +11541,9 @@
       <c r="A95" s="4" t="s">
         <v>694</v>
       </c>
-      <c r="B95" s="4"/>
+      <c r="B95" s="4" t="s">
+        <v>1487</v>
+      </c>
       <c r="C95" s="4" t="s">
         <v>695</v>
       </c>
@@ -11523,7 +11665,9 @@
       <c r="A97" s="4" t="s">
         <v>716</v>
       </c>
-      <c r="B97" s="4"/>
+      <c r="B97" s="4" t="s">
+        <v>1488</v>
+      </c>
       <c r="C97" s="4" t="s">
         <v>441</v>
       </c>
@@ -11584,7 +11728,9 @@
     </row>
     <row r="98" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
-      <c r="B98" s="4"/>
+      <c r="B98" s="4" t="s">
+        <v>725</v>
+      </c>
       <c r="C98" s="4" t="s">
         <v>725</v>
       </c>
@@ -11633,7 +11779,9 @@
     </row>
     <row r="99" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
-      <c r="B99" s="4"/>
+      <c r="B99" s="4" t="s">
+        <v>730</v>
+      </c>
       <c r="C99" s="4" t="s">
         <v>730</v>
       </c>
@@ -11680,7 +11828,9 @@
     </row>
     <row r="100" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
-      <c r="B100" s="4"/>
+      <c r="B100" s="4" t="s">
+        <v>735</v>
+      </c>
       <c r="C100" s="4" t="s">
         <v>735</v>
       </c>
@@ -11722,6 +11872,9 @@
       <c r="W100" s="7"/>
     </row>
     <row r="101" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>742</v>
+      </c>
       <c r="C101" t="s">
         <v>742</v>
       </c>
@@ -11754,6 +11907,9 @@
       </c>
     </row>
     <row r="102" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>746</v>
+      </c>
       <c r="C102" t="s">
         <v>746</v>
       </c>
@@ -11784,6 +11940,9 @@
       <c r="W102" s="3"/>
     </row>
     <row r="103" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>750</v>
+      </c>
       <c r="C103" t="s">
         <v>750</v>
       </c>
@@ -11909,7 +12068,9 @@
       <c r="A106" s="21" t="s">
         <v>768</v>
       </c>
-      <c r="B106" s="22"/>
+      <c r="B106" s="22" t="s">
+        <v>1486</v>
+      </c>
       <c r="C106" s="22" t="s">
         <v>441</v>
       </c>
@@ -12025,7 +12186,9 @@
       <c r="A108" s="21" t="s">
         <v>783</v>
       </c>
-      <c r="B108" s="22"/>
+      <c r="B108" s="22" t="s">
+        <v>1485</v>
+      </c>
       <c r="C108" s="22" t="s">
         <v>784</v>
       </c>
@@ -12094,7 +12257,9 @@
       <c r="A109" s="18" t="s">
         <v>794</v>
       </c>
-      <c r="B109" s="19"/>
+      <c r="B109" s="19" t="s">
+        <v>1484</v>
+      </c>
       <c r="C109" s="19" t="s">
         <v>502</v>
       </c>
@@ -12143,7 +12308,7 @@
       <c r="R109" s="19" t="s">
         <v>802</v>
       </c>
-      <c r="S109" s="19" t="s">
+      <c r="S109" s="46" t="s">
         <v>803</v>
       </c>
       <c r="T109" s="19" t="s">
@@ -12161,7 +12326,9 @@
       <c r="A110" s="21" t="s">
         <v>805</v>
       </c>
-      <c r="B110" s="22"/>
+      <c r="B110" s="22" t="s">
+        <v>1483</v>
+      </c>
       <c r="C110" s="22" t="s">
         <v>502</v>
       </c>
@@ -12220,7 +12387,9 @@
       <c r="A111" s="18" t="s">
         <v>814</v>
       </c>
-      <c r="B111" s="19"/>
+      <c r="B111" s="19" t="s">
+        <v>1482</v>
+      </c>
       <c r="C111" s="19" t="s">
         <v>813</v>
       </c>
@@ -12287,7 +12456,9 @@
       <c r="A112" s="21" t="s">
         <v>823</v>
       </c>
-      <c r="B112" s="22"/>
+      <c r="B112" s="22" t="s">
+        <v>1481</v>
+      </c>
       <c r="C112" s="22" t="s">
         <v>170</v>
       </c>
@@ -12336,7 +12507,7 @@
       <c r="R112" s="22" t="s">
         <v>802</v>
       </c>
-      <c r="S112" s="22" t="s">
+      <c r="S112" s="53" t="s">
         <v>832</v>
       </c>
       <c r="T112" s="22" t="s">
@@ -12356,7 +12527,9 @@
       <c r="A113" s="18" t="s">
         <v>834</v>
       </c>
-      <c r="B113" s="19"/>
+      <c r="B113" s="19" t="s">
+        <v>1480</v>
+      </c>
       <c r="C113" s="19" t="s">
         <v>835</v>
       </c>
@@ -12399,7 +12572,7 @@
       <c r="R113" s="19" t="s">
         <v>810</v>
       </c>
-      <c r="S113" s="19" t="s">
+      <c r="S113" s="46" t="s">
         <v>839</v>
       </c>
       <c r="T113" s="19" t="s">
@@ -12545,7 +12718,9 @@
       <c r="A116" s="21" t="s">
         <v>859</v>
       </c>
-      <c r="B116" s="22"/>
+      <c r="B116" s="22" t="s">
+        <v>1479</v>
+      </c>
       <c r="C116" s="22" t="s">
         <v>860</v>
       </c>
@@ -12588,7 +12763,7 @@
       <c r="R116" s="22" t="s">
         <v>774</v>
       </c>
-      <c r="S116" s="22" t="s">
+      <c r="S116" s="53" t="s">
         <v>864</v>
       </c>
       <c r="T116" s="22" t="s">
@@ -12608,7 +12783,9 @@
       <c r="A117" s="18" t="s">
         <v>867</v>
       </c>
-      <c r="B117" s="19"/>
+      <c r="B117" s="54" t="s">
+        <v>1478</v>
+      </c>
       <c r="C117" s="19" t="s">
         <v>860</v>
       </c>
@@ -12653,7 +12830,7 @@
       <c r="R117" s="19" t="s">
         <v>873</v>
       </c>
-      <c r="S117" s="19" t="s">
+      <c r="S117" s="46" t="s">
         <v>874</v>
       </c>
       <c r="T117" s="32" t="s">
@@ -12671,7 +12848,9 @@
       <c r="A118" s="21" t="s">
         <v>876</v>
       </c>
-      <c r="B118" s="22"/>
+      <c r="B118" s="55" t="s">
+        <v>1477</v>
+      </c>
       <c r="C118" s="22" t="s">
         <v>860</v>
       </c>
@@ -12783,7 +12962,9 @@
       <c r="A120" s="21" t="s">
         <v>888</v>
       </c>
-      <c r="B120" s="22"/>
+      <c r="B120" s="55" t="s">
+        <v>1476</v>
+      </c>
       <c r="C120" s="22" t="s">
         <v>161</v>
       </c>
@@ -12850,7 +13031,9 @@
       <c r="A121" s="18" t="s">
         <v>898</v>
       </c>
-      <c r="B121" s="19"/>
+      <c r="B121" s="54" t="s">
+        <v>1475</v>
+      </c>
       <c r="C121" s="19" t="s">
         <v>899</v>
       </c>
@@ -12915,7 +13098,9 @@
       <c r="A122" s="21" t="s">
         <v>906</v>
       </c>
-      <c r="B122" s="22"/>
+      <c r="B122" s="55" t="s">
+        <v>1474</v>
+      </c>
       <c r="C122" s="22" t="s">
         <v>263</v>
       </c>
@@ -13230,7 +13415,9 @@
       <c r="A127" s="18" t="s">
         <v>943</v>
       </c>
-      <c r="B127" s="19"/>
+      <c r="B127" s="54" t="s">
+        <v>1469</v>
+      </c>
       <c r="C127" s="19" t="s">
         <v>324</v>
       </c>
@@ -13295,7 +13482,9 @@
       <c r="A128" s="18" t="s">
         <v>952</v>
       </c>
-      <c r="B128" s="19"/>
+      <c r="B128" s="54" t="s">
+        <v>1473</v>
+      </c>
       <c r="C128" s="19" t="s">
         <v>953</v>
       </c>
@@ -13356,7 +13545,9 @@
       <c r="A129" s="21" t="s">
         <v>960</v>
       </c>
-      <c r="B129" s="22"/>
+      <c r="B129" s="55" t="s">
+        <v>1472</v>
+      </c>
       <c r="C129" s="22" t="s">
         <v>431</v>
       </c>
@@ -13405,7 +13596,7 @@
       <c r="R129" s="22" t="s">
         <v>802</v>
       </c>
-      <c r="S129" s="22" t="s">
+      <c r="S129" s="53" t="s">
         <v>967</v>
       </c>
       <c r="T129" s="22" t="s">
@@ -13423,7 +13614,9 @@
       <c r="A130" s="18" t="s">
         <v>969</v>
       </c>
-      <c r="B130" s="19"/>
+      <c r="B130" s="54" t="s">
+        <v>1471</v>
+      </c>
       <c r="C130" s="19" t="s">
         <v>431</v>
       </c>
@@ -13488,7 +13681,9 @@
       <c r="A131" s="21" t="s">
         <v>978</v>
       </c>
-      <c r="B131" s="22"/>
+      <c r="B131" s="55" t="s">
+        <v>1470</v>
+      </c>
       <c r="C131" s="22" t="s">
         <v>979</v>
       </c>
@@ -13610,7 +13805,9 @@
       <c r="A133" s="21" t="s">
         <v>995</v>
       </c>
-      <c r="B133" s="22"/>
+      <c r="B133" s="55" t="s">
+        <v>1468</v>
+      </c>
       <c r="C133" s="22" t="s">
         <v>996</v>
       </c>
@@ -13893,6 +14090,9 @@
       </c>
     </row>
     <row r="138" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>1497</v>
+      </c>
       <c r="C138" s="51" t="s">
         <v>1419</v>
       </c>

</xml_diff>

<commit_message>
Show a load status
</commit_message>
<xml_diff>
--- a/loadDatabase/religion/святые.xlsx
+++ b/loadDatabase/religion/святые.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18675" windowHeight="6675" tabRatio="587"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22635" windowHeight="7260" tabRatio="587"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2213" uniqueCount="1501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2241" uniqueCount="1514">
   <si>
     <t>Фамилия</t>
   </si>
@@ -5614,6 +5614,48 @@
   </si>
   <si>
     <t>3;9;15</t>
+  </si>
+  <si>
+    <t>Кирилл Просвятитель Славян</t>
+  </si>
+  <si>
+    <t>24.05</t>
+  </si>
+  <si>
+    <t>монах</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/0/06/Detail_of_Saint_Cyrill_statue_in_T%C5%99eb%C3%AD%C4%8D%2C_T%C5%99eb%C3%AD%C4%8D_District.jpg/800px-Detail_of_Saint_Cyrill_statue_in_T%C5%99eb%C3%AD%C4%8D%2C_T%C5%99eb%C3%AD%C4%8D_District.jpg</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Святой_Кирилл</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Родился в Фессалониках в семье полкового командира друнгария Льва, сына попавшего в опалу и сосланного в Фессалию столичного вельможи, но в 12 лет осиротел и стал воспитанником влиятельного логофета Феоктиста, опекуна малолетнего императора Михаила III. Проявив еще в детстве выдающиеся способности, обучался у лучших учителей Константинополя философии, диалектике, геометрии, арифметике, риторике, астрономии, а также разным языкам. По окончании учения, отказавшись заключить весьма выгодный брак с крестницей логофета Ириной, был посвящён во чтеца и поступил на службу хартофилаксом (буквально «хранителем библиотеки»; реально это равнялось современному званию академика) при соборе Святой Софии в Константинополе. На одном из богословских диспутов Кирилл одержал блестящую победу над многоопытным вождём иконоборцев, бывшим патриархом Иоанном VII «Аннием», что принесло ему широкую известность в столице. В 852 году (по другим данным, в 855-м) был отправлен в Багдад ко двору аббасидского халифа Аль-Мутаваккиля для диспута с мусульманскими богословами, оказавшими ему уважение и отдавшими должное его учености и знанию Корана. В 856 году логофет Феоктист, бывший покровителем Константина, был убит. Константин вместе со своими учениками Климентом, Наумом и Ангеларием пришёл в монастырь, где был настоятелем его брат Мефодий. В этом монастыре вокруг Константина и Мефодия сложилась группа единомышленников и зародилась мысль о создании славянской азбуки. В 862 году в Константинополь явились послы от великоморавского князя Ростислава с просьбой прислать учителей, которые «могли бы объяснить нам веру на нашем родном языке». Император и патриарх, призвав солунских братьев, предложили им идти к моравам. В Великой Моравии Константин и Мефодий продолжали переводить церковные книги с греческого на славянский язык, обучали славян чтению, письму и ведению богослужения на славянском языке. Братья пробыли в Великой Моравии более трёх лет, а затем отправились с учениками в Рим к папе Римскому. Среди части богословов Западной Церкви сложилась точка зрения, что хвала Богу может воздаваться только на трёх языках, на которых была сделана надпись на Кресте Господнем: еврейском, греческом и латинском. Поэтому Константин и Мефодий, проповедовавшие христианство в Моравии, были восприняты как еретики и вызваны в Рим. Там они надеялись найти поддержку в борьбе против немецкого духовенства, не желавшего сдавать свои позиции в Моравии и препятствовавшего распространению славянской письменности. По дороге в Рим посетили они ещё одну славянскую страну — Паннонию, где находилось Блатенское княжество. Здесь, в Блатнограде, по поручению князя Коцела братья обучали славян книжному делу и богослужению на славянском языке. После того, как Константин передал папе Римскому Адриану II обретённые им в своём херсонесском путешествии мощи святого Климента, тот утвердил богослужение на славянском языке, и переведённые книги приказал положить в римских церквях. Мефодий был рукоположён в епископский сан. В Риме Константин тяжело заболел, в начале декабря 868 года окончательно слёг, принял схиму и новое монашеское имя Кирилл, и через 50 дней (14 февраля) скончался. Перед смертью он сказал Мефодию: «Мы с тобой, как два вола; от тяжёлой ноши один упал, другой должен продолжать путь». Похоронен в Риме в церкви Святого Климента.
+</t>
+  </si>
+  <si>
+    <t>Мефодий Просвятитель Славян</t>
+  </si>
+  <si>
+    <t>Кирилл</t>
+  </si>
+  <si>
+    <t>Мефодий</t>
+  </si>
+  <si>
+    <t>Велеград, Чехия</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/4/42/Detail_of_Saint_Methodius_statue_in_T%C5%99eb%C3%AD%C4%8D%2C_T%C5%99eb%C3%AD%C4%8D_District.jpg/800px-Detail_of_Saint_Methodius_statue_in_T%C5%99eb%C3%AD%C4%8D%2C_T%C5%99eb%C3%AD%C4%8D_District.jpg</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Мефодий_Моравский</t>
+  </si>
+  <si>
+    <t>Происходит из семьи солунского военачальника, друнгария Льва. Учёным не известно, было ли имя Мефодий крещальным или дано при постриге. На православных сайтах приводится, что его мирским именем могло быть имя Михаил, не приводя при этом доказательств. Пользуясь поддержкой друга и покровителя семьи, великого логофета евнуха Феоктиста, сделал военно-административную карьеру, увенчавшуюся постом стратига Славинии, византийской провинции, расположенной на территории Македонии, где жили славяне. Он знал язык своих славянских подданных. В обители постников, которая называлась Малый Олимп и располагалась в Малой Азии, Мефодий принял монашество, позже здесь к нему присоединился и его брат Константин.
+Моравская миссия
+В 862 году в Константинополь явились послы от великоморавского князя Ростислава с просьбой прислать учителей. Император и патриарх, призвав солунских братьев, отправили их к моравам. Франкские епископы, прибывшие в Великую Моравию для обращения христиан к римским обычаям, арестовали Мефодия и посадили его в темницу. Никто не беспокоился о нём, и прошло почти три года, прежде чем Папа римский узнал о его судьбе и приказал Людовику Немецкому освободить его.</t>
   </si>
 </sst>
 </file>
@@ -6210,11 +6252,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X140"/>
+  <dimension ref="A1:X142"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="S1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S142" sqref="S142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14339,6 +14381,115 @@
       </c>
       <c r="X140" t="s">
         <v>1444</v>
+      </c>
+    </row>
+    <row r="141" spans="1:24" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>1501</v>
+      </c>
+      <c r="C141" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="E141" s="3">
+        <v>827</v>
+      </c>
+      <c r="F141" s="45" t="s">
+        <v>406</v>
+      </c>
+      <c r="H141" t="s">
+        <v>1508</v>
+      </c>
+      <c r="I141" t="s">
+        <v>677</v>
+      </c>
+      <c r="J141" s="3">
+        <v>852</v>
+      </c>
+      <c r="K141" t="s">
+        <v>42</v>
+      </c>
+      <c r="L141" s="3">
+        <v>862</v>
+      </c>
+      <c r="M141" t="s">
+        <v>18</v>
+      </c>
+      <c r="P141" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q141" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="R141" s="40" t="s">
+        <v>1502</v>
+      </c>
+      <c r="S141" s="45" t="s">
+        <v>1503</v>
+      </c>
+      <c r="T141" s="2" t="s">
+        <v>1506</v>
+      </c>
+      <c r="U141" s="1" t="s">
+        <v>1505</v>
+      </c>
+      <c r="V141" s="1" t="s">
+        <v>1504</v>
+      </c>
+      <c r="W141" s="3">
+        <v>869</v>
+      </c>
+      <c r="X141" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="142" spans="1:24" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>1507</v>
+      </c>
+      <c r="C142" s="52" t="s">
+        <v>263</v>
+      </c>
+      <c r="E142" s="3">
+        <v>815</v>
+      </c>
+      <c r="F142" s="45" t="s">
+        <v>406</v>
+      </c>
+      <c r="H142" t="s">
+        <v>1509</v>
+      </c>
+      <c r="I142" t="s">
+        <v>42</v>
+      </c>
+      <c r="J142" s="3">
+        <v>862</v>
+      </c>
+      <c r="P142" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q142" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="R142" s="40" t="s">
+        <v>1502</v>
+      </c>
+      <c r="S142" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="T142" s="2" t="s">
+        <v>1513</v>
+      </c>
+      <c r="U142" s="1" t="s">
+        <v>1512</v>
+      </c>
+      <c r="V142" s="1" t="s">
+        <v>1511</v>
+      </c>
+      <c r="W142" s="3">
+        <v>885</v>
+      </c>
+      <c r="X142" t="s">
+        <v>1510</v>
       </c>
     </row>
   </sheetData>
@@ -14589,9 +14740,13 @@
     <hyperlink ref="U105" r:id="rId242"/>
     <hyperlink ref="U136" r:id="rId243"/>
     <hyperlink ref="V134" r:id="rId244"/>
+    <hyperlink ref="V141" r:id="rId245"/>
+    <hyperlink ref="U141" r:id="rId246"/>
+    <hyperlink ref="V142" r:id="rId247"/>
+    <hyperlink ref="U142" r:id="rId248"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId245"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId249"/>
 </worksheet>
 </file>
 

</xml_diff>